<commit_message>
added controls from tripfolder page for parsing trip parameters
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="124">
   <si>
     <t>Description</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>12|20|22</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -1211,9 +1214,9 @@
   <dimension ref="A1:O89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection pane="topRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,10 +1293,10 @@
         <v>35</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="16">
-        <v>25</v>
+        <v>115</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="E2" s="6">
         <v>1</v>

</xml_diff>

<commit_message>
Completed airFlow without postSearchFilters
1. Added BfcPaymentPage
2. Added Payment Mode Parsing
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="109">
   <si>
     <t>Description</t>
   </si>
@@ -87,9 +87,6 @@
     <t>AmadeusWS air oneway booking for DOMESTIC location for 1 Adult with Login</t>
   </si>
   <si>
-    <t>AmadeusWS air oneway booking for DOMESTIC location for 1 Child with Login.</t>
-  </si>
-  <si>
     <t>AmadeusWS air oneway booking for DOMESTIC location for 1 Adult and 1 child with Login.</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult with Login.</t>
   </si>
   <si>
-    <t>AmadeusWS air round trip booking for DOMESTIC location for 1 Child with Login.</t>
-  </si>
-  <si>
     <t>AmadeusWS air round trip booking for DOMESTIC location for 1 adult and 1 child with Login.</t>
   </si>
   <si>
@@ -117,9 +111,6 @@
     <t>AmadeusWS air MULTICITY booking for DOMESTIC location for 1 Adult with Login.</t>
   </si>
   <si>
-    <t>AmadeusWS air MULTICITY booking for DOMESTIC location for 1 Child with Login.</t>
-  </si>
-  <si>
     <t>AmadeusWS air MULTICITY booking for DOMESTIC location 1 Adult and 1 child with Login.</t>
   </si>
   <si>
@@ -144,9 +135,6 @@
     <t>AmadeusWS air oneway booking for INTERNATIONAL location for 1 Adult with Login.</t>
   </si>
   <si>
-    <t>AmadeusWS air oneway booking for INTERNATIONAL location for 1 Child with Login.</t>
-  </si>
-  <si>
     <t>AmadeusWS air oneway booking for INTERNATIONAL location 1 Adult and 1 child with Login.</t>
   </si>
   <si>
@@ -165,9 +153,6 @@
     <t>Sabre air oneway booking for DOMESTIC location for 1 Adult with On Account payment mode</t>
   </si>
   <si>
-    <t>Sabre air oneway booking for DOMESTIC location for 1 Child with On Account payment mode</t>
-  </si>
-  <si>
     <t>Sabre air oneway booking for DOMESTIC location 1 Adult and 1 child with On Account payment mode</t>
   </si>
   <si>
@@ -180,9 +165,6 @@
     <t>Sabre air round trip booking for DOMESTIC location for 1 Adult with On Account payment mode</t>
   </si>
   <si>
-    <t>Sabre air round trip booking for DOMESTIC location for 1 Child with On Account payment mode</t>
-  </si>
-  <si>
     <t>Sabre air round trip booking for DOMESTIC location for 1 adult and 1 child with On Account payment mode</t>
   </si>
   <si>
@@ -195,9 +177,6 @@
     <t>Sabre air MULTICITY booking for DOMESTIC location for 1 Adult with On Account payment mode</t>
   </si>
   <si>
-    <t>Sabre air MULTICITY booking for DOMESTIC location for 1 Child with On Account payment mode</t>
-  </si>
-  <si>
     <t>Sabre air MULTICITY booking for DOMESTIC location 1 Adult and 1 child with On Account payment mode</t>
   </si>
   <si>
@@ -210,9 +189,6 @@
     <t>Sabre air oneway booking for INTERNATIONAL location for 1 Adult with On Account payment mode</t>
   </si>
   <si>
-    <t>Sabre air oneway booking for INTERNATIONAL location for 1 Child with On Account payment mode</t>
-  </si>
-  <si>
     <t>Sabre air oneway booking for INTERNATIONAL location 1 Adult and 1 child with On Account payment mode</t>
   </si>
   <si>
@@ -231,9 +207,6 @@
     <t>Worldspan air oneway booking for DOMESTIC location for 1 Adult with With_Login payment mode.</t>
   </si>
   <si>
-    <t>Worldspan air oneway booking for DOMESTIC location 1 Child with OnAccount payment mode.</t>
-  </si>
-  <si>
     <t>Worldspan air oneway booking for DOMESTIC location 1 Adult and 1 child with OnAccount payment mode.</t>
   </si>
   <si>
@@ -246,9 +219,6 @@
     <t>Worldspan air round trip booking for DOMESTIC location for 1 Adult with OnAccount payment mode.</t>
   </si>
   <si>
-    <t>Worldspan air round trip booking for DOMESTIC location for 1 Child with OnAccount payment mode.</t>
-  </si>
-  <si>
     <t>Worldspan air round trip booking for DOMESTIC location 1 Adult and 1 child with OnAccount payment mode.</t>
   </si>
   <si>
@@ -261,9 +231,6 @@
     <t>Worldspan air MULTICITY booking for DOMESTIC location for 1 Adult with OnAccount payment mode.</t>
   </si>
   <si>
-    <t>Worldspan air MULTICITY booking for DOMESTIC location for 1 Child with OnAccount payment mode.</t>
-  </si>
-  <si>
     <t>Worldspan air MULTICITY booking for DOMESTIC location 1 Adult and 1 child with OnAccount payment mode.</t>
   </si>
   <si>
@@ -276,9 +243,6 @@
     <t>Worldspan air oneway booking for INTERNATIONAL location for 1 Adult with OnAccount payment mode.</t>
   </si>
   <si>
-    <t>Worldspan air oneway booking for INTERNATIONAL location for 1 Child with OnAccount payment mode.</t>
-  </si>
-  <si>
     <t>Worldspan air oneway booking for INTERNATIONAL location 1 Adult and 1 child with OnAccount payment mode.</t>
   </si>
   <si>
@@ -297,9 +261,6 @@
     <t>MYSTIFLY air oneway booking for DOMESTIC location for 1 Adult with OnAccount payment mode.</t>
   </si>
   <si>
-    <t>MYSTIFLY air oneway booking for DOMESTIC location 1 Child with OnAccount payment mode.</t>
-  </si>
-  <si>
     <t>MYSTIFLY air oneway booking for DOMESTIC location 1 Adult and 1 child with OnAccount payment mode.</t>
   </si>
   <si>
@@ -312,9 +273,6 @@
     <t>MYSTIFLY air round trip booking for DOMESTIC location for 1 Adult with OnAccount payment mode.</t>
   </si>
   <si>
-    <t>MYSTIFLY air round trip booking for DOMESTIC location for 1 Child with OnAccount payment mode.</t>
-  </si>
-  <si>
     <t>MYSTIFLY air round trip booking for DOMESTIC location 1 Adult and 1 child with OnAccount payment mode.</t>
   </si>
   <si>
@@ -327,9 +285,6 @@
     <t>MYSTIFLY air MULTICITY booking for DOMESTIC location for 1 Adult with OnAccount payment mode.</t>
   </si>
   <si>
-    <t>MYSTIFLY air MULTICITY booking for DOMESTIC location for 1 Child with OnAccount payment mode.</t>
-  </si>
-  <si>
     <t>MYSTIFLY air MULTICITY booking for DOMESTIC location 1 Adult and 1 child with OnAccount payment mode.</t>
   </si>
   <si>
@@ -342,9 +297,6 @@
     <t>MYSTIFLY air oneway booking for INTERNATIONAL location for 1 Adult with OnAccount payment mode.</t>
   </si>
   <si>
-    <t>MYSTIFLY air oneway booking for INTERNATIONAL location for 1 Child with OnAccount payment mode.</t>
-  </si>
-  <si>
     <t>MYSTIFLY air oneway booking for INTERNATIONAL location 1 Adult and 1 child with OnAccount payment mode.</t>
   </si>
   <si>
@@ -388,6 +340,9 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>CreditCard|Visa</t>
   </si>
 </sst>
 </file>
@@ -901,8 +856,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:O89" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="A1:O89"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:O73" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:O73"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Description" dataDxfId="14"/>
     <tableColumn id="2" name="TripType" dataDxfId="13"/>
@@ -1211,12 +1166,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O89"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,13 +1245,13 @@
         <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="E2" s="6">
         <v>1</v>
@@ -1318,7 +1273,7 @@
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>20</v>
@@ -1327,7 +1282,7 @@
         <v>21</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -1335,7 +1290,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -1343,27 +1298,27 @@
       <c r="D3" s="16">
         <v>25</v>
       </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5" t="b">
+      <c r="E3" s="10">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10" t="b">
         <v>0</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5"/>
+      <c r="J3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="10"/>
       <c r="L3" s="8" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>20</v>
@@ -1372,7 +1327,7 @@
         <v>21</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -1380,7 +1335,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
@@ -1392,10 +1347,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="10" t="b">
         <v>0</v>
@@ -1408,7 +1363,7 @@
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="8" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>20</v>
@@ -1417,7 +1372,7 @@
         <v>21</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -1425,7 +1380,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>16</v>
@@ -1433,27 +1388,27 @@
       <c r="D5" s="16">
         <v>25</v>
       </c>
-      <c r="E5" s="10">
-        <v>1</v>
-      </c>
-      <c r="F5" s="10">
-        <v>1</v>
-      </c>
-      <c r="G5" s="10">
-        <v>0</v>
-      </c>
-      <c r="H5" s="10" t="b">
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="10"/>
+      <c r="J5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5"/>
       <c r="L5" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>20</v>
@@ -1462,32 +1417,32 @@
         <v>21</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>35</v>
+      <c r="B6" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="16">
-        <v>25</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5" t="b">
+      <c r="D6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I6" s="6" t="s">
@@ -1496,9 +1451,9 @@
       <c r="J6" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K6" s="5"/>
+      <c r="K6" s="10"/>
       <c r="L6" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>20</v>
@@ -1507,7 +1462,7 @@
         <v>21</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -1530,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="6" t="b">
         <v>0</v>
@@ -1543,7 +1498,7 @@
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>20</v>
@@ -1552,7 +1507,7 @@
         <v>21</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -1568,14 +1523,14 @@
       <c r="D8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="10">
-        <v>0</v>
-      </c>
-      <c r="F8" s="10">
-        <v>0</v>
-      </c>
-      <c r="G8" s="10">
-        <v>1</v>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
       </c>
       <c r="H8" s="6" t="b">
         <v>0</v>
@@ -1586,9 +1541,9 @@
       <c r="J8" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K8" s="10"/>
+      <c r="K8" s="5"/>
       <c r="L8" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M8" s="8" t="s">
         <v>20</v>
@@ -1597,7 +1552,7 @@
         <v>21</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -1613,13 +1568,13 @@
       <c r="D9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="10">
-        <v>1</v>
-      </c>
-      <c r="F9" s="10">
-        <v>0</v>
-      </c>
-      <c r="G9" s="10">
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
         <v>1</v>
       </c>
       <c r="H9" s="6" t="b">
@@ -1631,9 +1586,9 @@
       <c r="J9" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K9" s="10"/>
+      <c r="K9" s="5"/>
       <c r="L9" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M9" s="8" t="s">
         <v>20</v>
@@ -1642,27 +1597,27 @@
         <v>21</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>17</v>
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
       </c>
       <c r="F10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="5">
         <v>0</v>
@@ -1678,7 +1633,7 @@
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>20</v>
@@ -1687,29 +1642,29 @@
         <v>21</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5">
+      <c r="B11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
         <v>1</v>
       </c>
       <c r="H11" s="6" t="b">
@@ -1721,9 +1676,9 @@
       <c r="J11" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K11" s="5"/>
+      <c r="K11" s="6"/>
       <c r="L11" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>20</v>
@@ -1732,27 +1687,27 @@
         <v>21</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>38</v>
+      <c r="A12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="E12" s="5">
         <v>1</v>
       </c>
       <c r="F12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="5">
         <v>0</v>
@@ -1768,7 +1723,7 @@
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M12" s="8" t="s">
         <v>20</v>
@@ -1777,27 +1732,27 @@
         <v>21</v>
       </c>
       <c r="O12" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>38</v>
+      <c r="B13" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="E13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="5">
         <v>1</v>
@@ -1813,7 +1768,7 @@
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M13" s="8" t="s">
         <v>20</v>
@@ -1822,30 +1777,30 @@
         <v>21</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="12" t="s">
         <v>38</v>
       </c>
+      <c r="B14" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="C14" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D14" s="16">
+        <v>25</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
       </c>
       <c r="H14" s="6" t="b">
         <v>0</v>
@@ -1856,9 +1811,9 @@
       <c r="J14" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="5"/>
       <c r="L14" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M14" s="8" t="s">
         <v>20</v>
@@ -1867,7 +1822,7 @@
         <v>21</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -1875,22 +1830,22 @@
         <v>39</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>120</v>
+        <v>98</v>
+      </c>
+      <c r="D15" s="16">
+        <v>25</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
       </c>
       <c r="F15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="6" t="b">
         <v>0</v>
@@ -1903,7 +1858,7 @@
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>20</v>
@@ -1912,7 +1867,7 @@
         <v>21</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -1920,13 +1875,13 @@
         <v>40</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>120</v>
+        <v>98</v>
+      </c>
+      <c r="D16" s="16">
+        <v>25</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
@@ -1935,7 +1890,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="6" t="b">
         <v>0</v>
@@ -1948,7 +1903,7 @@
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>20</v>
@@ -1957,30 +1912,30 @@
         <v>21</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>35</v>
+      <c r="B17" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D17" s="16">
         <v>25</v>
       </c>
-      <c r="E17" s="5">
-        <v>1</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0</v>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
       </c>
       <c r="H17" s="6" t="b">
         <v>0</v>
@@ -1991,9 +1946,9 @@
       <c r="J17" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K17" s="5"/>
+      <c r="K17" s="6"/>
       <c r="L17" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M17" s="8" t="s">
         <v>20</v>
@@ -2002,7 +1957,7 @@
         <v>21</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2010,22 +1965,22 @@
         <v>42</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D18" s="16">
-        <v>25</v>
+        <v>98</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="5">
         <v>0</v>
       </c>
       <c r="G18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="6" t="b">
         <v>0</v>
@@ -2038,7 +1993,7 @@
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M18" s="8" t="s">
         <v>20</v>
@@ -2047,7 +2002,7 @@
         <v>21</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2058,10 +2013,10 @@
         <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="16">
-        <v>25</v>
+        <v>105</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>106</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
@@ -2070,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="6" t="b">
         <v>0</v>
@@ -2083,7 +2038,7 @@
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M19" s="8" t="s">
         <v>20</v>
@@ -2092,7 +2047,7 @@
         <v>21</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2100,10 +2055,10 @@
         <v>44</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D20" s="16">
         <v>25</v>
@@ -2112,7 +2067,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="5">
         <v>0</v>
@@ -2126,40 +2081,42 @@
       <c r="J20" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="L20" s="8" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="M20" s="8" t="s">
         <v>20</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>35</v>
+      <c r="B21" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D21" s="16">
         <v>25</v>
       </c>
-      <c r="E21" s="6">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1</v>
-      </c>
-      <c r="G21" s="6">
+      <c r="E21" s="5">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
         <v>1</v>
       </c>
       <c r="H21" s="6" t="b">
@@ -2171,40 +2128,42 @@
       <c r="J21" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K21" s="6"/>
+      <c r="K21" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="L21" s="8" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="M21" s="8" t="s">
         <v>20</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>15</v>
+      <c r="B22" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="5">
-        <v>1</v>
-      </c>
-      <c r="F22" s="5">
-        <v>0</v>
-      </c>
-      <c r="G22" s="5">
+        <v>99</v>
+      </c>
+      <c r="D22" s="16">
+        <v>25</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
+        <v>1</v>
+      </c>
+      <c r="G22" s="6">
         <v>0</v>
       </c>
       <c r="H22" s="6" t="b">
@@ -2216,18 +2175,20 @@
       <c r="J22" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K22" s="5"/>
+      <c r="K22" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="L22" s="8" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="M22" s="8" t="s">
         <v>20</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2235,22 +2196,22 @@
         <v>47</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>122</v>
+        <v>99</v>
+      </c>
+      <c r="D23" s="16">
+        <v>25</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
       </c>
       <c r="F23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="6" t="b">
         <v>0</v>
@@ -2261,18 +2222,20 @@
       <c r="J23" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K23" s="5"/>
+      <c r="K23" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="L23" s="8" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="M23" s="8" t="s">
         <v>20</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2280,13 +2243,13 @@
         <v>48</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D24" s="16">
-        <v>25</v>
+        <v>99</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
@@ -2307,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>19</v>
@@ -2316,10 +2279,10 @@
         <v>20</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2327,16 +2290,16 @@
         <v>49</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="16">
-        <v>25</v>
+        <v>99</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="5">
         <v>0</v>
@@ -2354,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>19</v>
@@ -2363,10 +2326,10 @@
         <v>20</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2374,22 +2337,22 @@
         <v>50</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D26" s="16">
-        <v>25</v>
+        <v>99</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
       </c>
       <c r="F26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="6" t="b">
         <v>0</v>
@@ -2401,7 +2364,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>19</v>
@@ -2410,33 +2373,33 @@
         <v>20</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>35</v>
+      <c r="B27" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="16">
-        <v>25</v>
-      </c>
-      <c r="E27" s="6">
-        <v>1</v>
-      </c>
-      <c r="F27" s="6">
-        <v>1</v>
-      </c>
-      <c r="G27" s="6">
-        <v>0</v>
+        <v>99</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="5">
+        <v>1</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
+      <c r="G27" s="5">
+        <v>1</v>
       </c>
       <c r="H27" s="6" t="b">
         <v>0</v>
@@ -2448,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>19</v>
@@ -2457,10 +2420,10 @@
         <v>20</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2471,19 +2434,19 @@
         <v>35</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="16">
-        <v>25</v>
+        <v>103</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
       </c>
       <c r="F28" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="6" t="b">
         <v>0</v>
@@ -2495,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>19</v>
@@ -2504,10 +2467,10 @@
         <v>20</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2515,13 +2478,13 @@
         <v>53</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>17</v>
+        <v>103</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="E29" s="5">
         <v>1</v>
@@ -2530,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="6" t="b">
         <v>0</v>
@@ -2542,7 +2505,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L29" s="8" t="s">
         <v>19</v>
@@ -2551,10 +2514,10 @@
         <v>20</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2562,22 +2525,22 @@
         <v>54</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>17</v>
+        <v>103</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="E30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="6" t="b">
         <v>0</v>
@@ -2589,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>19</v>
@@ -2598,30 +2561,30 @@
         <v>20</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>17</v>
+        <v>103</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="E31" s="5">
         <v>1</v>
       </c>
       <c r="F31" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="5">
         <v>1</v>
@@ -2636,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>19</v>
@@ -2645,10 +2608,10 @@
         <v>20</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2656,19 +2619,19 @@
         <v>56</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>17</v>
+        <v>99</v>
+      </c>
+      <c r="D32" s="16">
+        <v>25</v>
       </c>
       <c r="E32" s="5">
         <v>1</v>
       </c>
       <c r="F32" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="5">
         <v>0</v>
@@ -2683,7 +2646,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>19</v>
@@ -2692,30 +2655,30 @@
         <v>20</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>17</v>
+        <v>99</v>
+      </c>
+      <c r="D33" s="16">
+        <v>25</v>
       </c>
       <c r="E33" s="5">
         <v>1</v>
       </c>
       <c r="F33" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="5">
         <v>1</v>
@@ -2730,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L33" s="8" t="s">
         <v>19</v>
@@ -2739,10 +2702,10 @@
         <v>20</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2750,19 +2713,19 @@
         <v>58</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>120</v>
+        <v>99</v>
+      </c>
+      <c r="D34" s="16">
+        <v>25</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
       </c>
       <c r="F34" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="5">
         <v>0</v>
@@ -2777,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L34" s="8" t="s">
         <v>19</v>
@@ -2786,32 +2749,32 @@
         <v>20</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>38</v>
+      <c r="B35" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="E35" s="6">
-        <v>0</v>
-      </c>
-      <c r="F35" s="6">
-        <v>0</v>
-      </c>
-      <c r="G35" s="6">
+        <v>99</v>
+      </c>
+      <c r="D35" s="16">
+        <v>25</v>
+      </c>
+      <c r="E35" s="5">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="5">
         <v>1</v>
       </c>
       <c r="H35" s="6" t="b">
@@ -2824,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L35" s="8" t="s">
         <v>19</v>
@@ -2833,33 +2796,33 @@
         <v>20</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>38</v>
+      <c r="B36" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="E36" s="5">
-        <v>1</v>
-      </c>
-      <c r="F36" s="5">
-        <v>0</v>
-      </c>
-      <c r="G36" s="5">
-        <v>1</v>
+        <v>99</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="6">
+        <v>1</v>
+      </c>
+      <c r="F36" s="6">
+        <v>0</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0</v>
       </c>
       <c r="H36" s="6" t="b">
         <v>0</v>
@@ -2871,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L36" s="8" t="s">
         <v>19</v>
@@ -2880,10 +2843,10 @@
         <v>20</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O36" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -2891,19 +2854,19 @@
         <v>61</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="E37" s="5">
         <v>1</v>
       </c>
       <c r="F37" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" s="5">
         <v>0</v>
@@ -2918,7 +2881,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="L37" s="8" t="s">
         <v>19</v>
@@ -2927,33 +2890,33 @@
         <v>20</v>
       </c>
       <c r="N37" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>120</v>
+        <v>99</v>
+      </c>
+      <c r="D38" s="16">
+        <v>25</v>
       </c>
       <c r="E38" s="5">
         <v>1</v>
       </c>
       <c r="F38" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" s="6" t="b">
         <v>0</v>
@@ -2964,9 +2927,7 @@
       <c r="J38" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K38" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="K38" s="5"/>
       <c r="L38" s="8" t="s">
         <v>19</v>
       </c>
@@ -2974,21 +2935,21 @@
         <v>20</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D39" s="16">
         <v>25</v>
@@ -3000,7 +2961,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="6" t="b">
         <v>0</v>
@@ -3011,9 +2972,7 @@
       <c r="J39" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K39" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="K39" s="5"/>
       <c r="L39" s="8" t="s">
         <v>19</v>
       </c>
@@ -3021,33 +2980,33 @@
         <v>20</v>
       </c>
       <c r="N39" s="8" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="O39" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>64</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D40" s="16">
         <v>25</v>
       </c>
       <c r="E40" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" s="6" t="b">
         <v>0</v>
@@ -3058,9 +3017,7 @@
       <c r="J40" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K40" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="K40" s="5"/>
       <c r="L40" s="8" t="s">
         <v>19</v>
       </c>
@@ -3068,21 +3025,21 @@
         <v>20</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="O40" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D41" s="16">
         <v>25</v>
@@ -3091,7 +3048,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="5">
         <v>1</v>
@@ -3105,9 +3062,7 @@
       <c r="J41" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K41" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="K41" s="5"/>
       <c r="L41" s="8" t="s">
         <v>19</v>
       </c>
@@ -3115,10 +3070,10 @@
         <v>20</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="O41" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -3126,19 +3081,19 @@
         <v>66</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" s="16">
-        <v>25</v>
+        <v>99</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E42" s="5">
         <v>1</v>
       </c>
       <c r="F42" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" s="5">
         <v>0</v>
@@ -3152,9 +3107,7 @@
       <c r="J42" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K42" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="K42" s="5"/>
       <c r="L42" s="8" t="s">
         <v>19</v>
       </c>
@@ -3162,10 +3115,10 @@
         <v>20</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="O42" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
@@ -3173,19 +3126,19 @@
         <v>67</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D43" s="16">
-        <v>25</v>
+        <v>99</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E43" s="5">
         <v>1</v>
       </c>
       <c r="F43" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="5">
         <v>1</v>
@@ -3199,9 +3152,7 @@
       <c r="J43" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K43" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="K43" s="5"/>
       <c r="L43" s="8" t="s">
         <v>19</v>
       </c>
@@ -3209,32 +3160,32 @@
         <v>20</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="O43" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="6">
-        <v>1</v>
-      </c>
-      <c r="F44" s="6">
-        <v>0</v>
-      </c>
-      <c r="G44" s="6">
+      <c r="E44" s="5">
+        <v>1</v>
+      </c>
+      <c r="F44" s="5">
+        <v>1</v>
+      </c>
+      <c r="G44" s="5">
         <v>0</v>
       </c>
       <c r="H44" s="6" t="b">
@@ -3246,9 +3197,7 @@
       <c r="J44" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K44" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="K44" s="5"/>
       <c r="L44" s="8" t="s">
         <v>19</v>
       </c>
@@ -3256,33 +3205,33 @@
         <v>20</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="O44" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>69</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>122</v>
+        <v>99</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E45" s="5">
         <v>1</v>
       </c>
       <c r="F45" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="6" t="b">
         <v>0</v>
@@ -3293,9 +3242,7 @@
       <c r="J45" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K45" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="K45" s="5"/>
       <c r="L45" s="8" t="s">
         <v>19</v>
       </c>
@@ -3303,10 +3250,10 @@
         <v>20</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -3316,12 +3263,8 @@
       <c r="B46" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D46" s="16">
-        <v>25</v>
-      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="15"/>
       <c r="E46" s="5">
         <v>1</v>
       </c>
@@ -3348,27 +3291,23 @@
         <v>20</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="O46" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>71</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D47" s="16">
-        <v>25</v>
-      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="15"/>
       <c r="E47" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" s="5">
         <v>0</v>
@@ -3393,10 +3332,10 @@
         <v>20</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="O47" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
@@ -3406,20 +3345,16 @@
       <c r="B48" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D48" s="16">
-        <v>25</v>
-      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="15"/>
       <c r="E48" s="5">
         <v>1</v>
       </c>
       <c r="F48" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" s="6" t="b">
         <v>0</v>
@@ -3438,10 +3373,10 @@
         <v>20</v>
       </c>
       <c r="N48" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="O48" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
@@ -3451,12 +3386,8 @@
       <c r="B49" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D49" s="16">
-        <v>25</v>
-      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="15"/>
       <c r="E49" s="5">
         <v>1</v>
       </c>
@@ -3464,7 +3395,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" s="6" t="b">
         <v>0</v>
@@ -3483,33 +3414,31 @@
         <v>20</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="O49" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="B50" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="6"/>
       <c r="D50" s="16">
         <v>25</v>
       </c>
-      <c r="E50" s="5">
-        <v>1</v>
-      </c>
-      <c r="F50" s="5">
-        <v>1</v>
-      </c>
-      <c r="G50" s="5">
-        <v>1</v>
+      <c r="E50" s="6">
+        <v>1</v>
+      </c>
+      <c r="F50" s="6">
+        <v>0</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0</v>
       </c>
       <c r="H50" s="6" t="b">
         <v>0</v>
@@ -3520,7 +3449,7 @@
       <c r="J50" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K50" s="5"/>
+      <c r="K50" s="6"/>
       <c r="L50" s="8" t="s">
         <v>19</v>
       </c>
@@ -3528,24 +3457,22 @@
         <v>20</v>
       </c>
       <c r="N50" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="O50" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>75</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="16">
+        <v>25</v>
       </c>
       <c r="E51" s="5">
         <v>1</v>
@@ -3554,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" s="6" t="b">
         <v>0</v>
@@ -3573,33 +3500,31 @@
         <v>20</v>
       </c>
       <c r="N51" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="O51" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E52" s="6">
-        <v>0</v>
-      </c>
-      <c r="F52" s="6">
-        <v>0</v>
-      </c>
-      <c r="G52" s="6">
-        <v>1</v>
+      <c r="B52" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="16">
+        <v>25</v>
+      </c>
+      <c r="E52" s="5">
+        <v>1</v>
+      </c>
+      <c r="F52" s="5">
+        <v>1</v>
+      </c>
+      <c r="G52" s="5">
+        <v>0</v>
       </c>
       <c r="H52" s="6" t="b">
         <v>0</v>
@@ -3610,7 +3535,7 @@
       <c r="J52" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K52" s="6"/>
+      <c r="K52" s="5"/>
       <c r="L52" s="8" t="s">
         <v>19</v>
       </c>
@@ -3618,10 +3543,10 @@
         <v>20</v>
       </c>
       <c r="N52" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="O52" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
@@ -3629,19 +3554,17 @@
         <v>77</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="16">
+        <v>25</v>
       </c>
       <c r="E53" s="5">
         <v>1</v>
       </c>
       <c r="F53" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="5">
         <v>1</v>
@@ -3663,22 +3586,20 @@
         <v>20</v>
       </c>
       <c r="N53" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="O53" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="C54" s="5"/>
       <c r="D54" s="17" t="s">
         <v>17</v>
       </c>
@@ -3686,7 +3607,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" s="5">
         <v>0</v>
@@ -3708,33 +3629,29 @@
         <v>20</v>
       </c>
       <c r="N54" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="O54" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B55" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>17</v>
-      </c>
+      <c r="B55" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="15"/>
       <c r="E55" s="5">
         <v>1</v>
       </c>
       <c r="F55" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55" s="6" t="b">
         <v>0</v>
@@ -3753,10 +3670,10 @@
         <v>20</v>
       </c>
       <c r="N55" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="O55" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -3764,10 +3681,12 @@
         <v>80</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C56" s="5"/>
-      <c r="D56" s="15"/>
+      <c r="D56" s="16">
+        <v>25</v>
+      </c>
       <c r="E56" s="5">
         <v>1</v>
       </c>
@@ -3793,24 +3712,24 @@
       <c r="M56" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N56" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N56" s="8"/>
       <c r="O56" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>81</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C57" s="5"/>
-      <c r="D57" s="15"/>
+      <c r="D57" s="16">
+        <v>25</v>
+      </c>
       <c r="E57" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57" s="5">
         <v>0</v>
@@ -3834,30 +3753,30 @@
       <c r="M57" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N57" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N57" s="8"/>
       <c r="O57" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B58" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="5">
-        <v>1</v>
-      </c>
-      <c r="F58" s="5">
-        <v>0</v>
-      </c>
-      <c r="G58" s="5">
-        <v>1</v>
+      <c r="B58" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="16">
+        <v>25</v>
+      </c>
+      <c r="E58" s="6">
+        <v>1</v>
+      </c>
+      <c r="F58" s="6">
+        <v>1</v>
+      </c>
+      <c r="G58" s="6">
+        <v>0</v>
       </c>
       <c r="H58" s="6" t="b">
         <v>0</v>
@@ -3868,18 +3787,16 @@
       <c r="J58" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K58" s="5"/>
+      <c r="K58" s="6"/>
       <c r="L58" s="8" t="s">
         <v>19</v>
       </c>
       <c r="M58" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N58" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N58" s="8"/>
       <c r="O58" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
@@ -3887,10 +3804,12 @@
         <v>83</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C59" s="5"/>
-      <c r="D59" s="15"/>
+      <c r="D59" s="16">
+        <v>25</v>
+      </c>
       <c r="E59" s="5">
         <v>1</v>
       </c>
@@ -3898,7 +3817,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" s="6" t="b">
         <v>0</v>
@@ -3916,30 +3835,30 @@
       <c r="M59" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N59" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N59" s="8"/>
       <c r="O59" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>84</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C60" s="5"/>
-      <c r="D60" s="15"/>
+      <c r="D60" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="E60" s="5">
         <v>1</v>
       </c>
       <c r="F60" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" s="6" t="b">
         <v>0</v>
@@ -3957,32 +3876,30 @@
       <c r="M60" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N60" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N60" s="8"/>
       <c r="O60" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="16">
-        <v>25</v>
-      </c>
-      <c r="E61" s="6">
-        <v>1</v>
-      </c>
-      <c r="F61" s="6">
-        <v>0</v>
-      </c>
-      <c r="G61" s="6">
-        <v>0</v>
+      <c r="B61" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="5">
+        <v>1</v>
+      </c>
+      <c r="F61" s="5">
+        <v>0</v>
+      </c>
+      <c r="G61" s="5">
+        <v>1</v>
       </c>
       <c r="H61" s="6" t="b">
         <v>0</v>
@@ -3993,39 +3910,37 @@
       <c r="J61" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K61" s="6"/>
+      <c r="K61" s="5"/>
       <c r="L61" s="8" t="s">
         <v>19</v>
       </c>
       <c r="M61" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N61" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N61" s="8"/>
       <c r="O61" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>86</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C62" s="5"/>
-      <c r="D62" s="16">
-        <v>25</v>
+      <c r="D62" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E62" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" s="6" t="b">
         <v>0</v>
@@ -4043,11 +3958,9 @@
       <c r="M62" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N62" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N62" s="8"/>
       <c r="O62" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
@@ -4055,17 +3968,17 @@
         <v>87</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C63" s="5"/>
-      <c r="D63" s="16">
-        <v>25</v>
+      <c r="D63" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E63" s="5">
         <v>1</v>
       </c>
       <c r="F63" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63" s="5">
         <v>1</v>
@@ -4086,14 +3999,12 @@
       <c r="M63" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N63" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N63" s="8"/>
       <c r="O63" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="51" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>88</v>
       </c>
@@ -4101,14 +4012,12 @@
         <v>35</v>
       </c>
       <c r="C64" s="5"/>
-      <c r="D64" s="16">
-        <v>25</v>
-      </c>
+      <c r="D64" s="15"/>
       <c r="E64" s="5">
         <v>1</v>
       </c>
       <c r="F64" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="5">
         <v>0</v>
@@ -4129,11 +4038,9 @@
       <c r="M64" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N64" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N64" s="8"/>
       <c r="O64" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
@@ -4144,14 +4051,12 @@
         <v>35</v>
       </c>
       <c r="C65" s="5"/>
-      <c r="D65" s="16">
-        <v>25</v>
-      </c>
+      <c r="D65" s="15"/>
       <c r="E65" s="5">
         <v>1</v>
       </c>
       <c r="F65" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" s="5">
         <v>1</v>
@@ -4172,29 +4077,25 @@
       <c r="M65" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N65" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N65" s="8"/>
       <c r="O65" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>90</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C66" s="5"/>
-      <c r="D66" s="17" t="s">
-        <v>17</v>
-      </c>
+      <c r="D66" s="15"/>
       <c r="E66" s="5">
         <v>1</v>
       </c>
       <c r="F66" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="5">
         <v>0</v>
@@ -4215,19 +4116,17 @@
       <c r="M66" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N66" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N66" s="8"/>
       <c r="O66" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>38</v>
+      <c r="B67" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="15"/>
@@ -4235,10 +4134,10 @@
         <v>1</v>
       </c>
       <c r="F67" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67" s="6" t="b">
         <v>0</v>
@@ -4256,11 +4155,9 @@
       <c r="M67" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N67" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="N67" s="8"/>
       <c r="O67" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="51" x14ac:dyDescent="0.25">
@@ -4268,7 +4165,7 @@
         <v>92</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="16">
@@ -4301,22 +4198,22 @@
       </c>
       <c r="N68" s="8"/>
       <c r="O68" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>93</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="16">
         <v>25</v>
       </c>
       <c r="E69" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" s="5">
         <v>0</v>
@@ -4342,7 +4239,7 @@
       </c>
       <c r="N69" s="8"/>
       <c r="O69" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
@@ -4350,7 +4247,7 @@
         <v>94</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="16">
@@ -4360,10 +4257,10 @@
         <v>1</v>
       </c>
       <c r="F70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G70" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70" s="6" t="b">
         <v>0</v>
@@ -4383,28 +4280,28 @@
       </c>
       <c r="N70" s="8"/>
       <c r="O70" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B71" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C71" s="6"/>
+      <c r="B71" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C71" s="5"/>
       <c r="D71" s="16">
         <v>25</v>
       </c>
-      <c r="E71" s="6">
-        <v>1</v>
-      </c>
-      <c r="F71" s="6">
-        <v>1</v>
-      </c>
-      <c r="G71" s="6">
-        <v>0</v>
+      <c r="E71" s="5">
+        <v>1</v>
+      </c>
+      <c r="F71" s="5">
+        <v>1</v>
+      </c>
+      <c r="G71" s="5">
+        <v>1</v>
       </c>
       <c r="H71" s="6" t="b">
         <v>0</v>
@@ -4415,7 +4312,7 @@
       <c r="J71" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K71" s="6"/>
+      <c r="K71" s="5"/>
       <c r="L71" s="8" t="s">
         <v>19</v>
       </c>
@@ -4424,28 +4321,28 @@
       </c>
       <c r="N71" s="8"/>
       <c r="O71" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="51" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B72" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="16">
-        <v>25</v>
-      </c>
-      <c r="E72" s="5">
-        <v>1</v>
-      </c>
-      <c r="F72" s="5">
-        <v>1</v>
-      </c>
-      <c r="G72" s="5">
-        <v>1</v>
+      <c r="B72" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" s="6">
+        <v>1</v>
+      </c>
+      <c r="F72" s="6">
+        <v>0</v>
+      </c>
+      <c r="G72" s="6">
+        <v>0</v>
       </c>
       <c r="H72" s="6" t="b">
         <v>0</v>
@@ -4456,7 +4353,7 @@
       <c r="J72" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K72" s="5"/>
+      <c r="K72" s="6"/>
       <c r="L72" s="8" t="s">
         <v>19</v>
       </c>
@@ -4465,27 +4362,25 @@
       </c>
       <c r="N72" s="8"/>
       <c r="O72" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B73" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E73" s="5">
-        <v>1</v>
-      </c>
-      <c r="F73" s="5">
-        <v>0</v>
-      </c>
-      <c r="G73" s="5">
+      <c r="B73" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" s="6"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="6">
+        <v>1</v>
+      </c>
+      <c r="F73" s="6">
+        <v>0</v>
+      </c>
+      <c r="G73" s="6">
         <v>0</v>
       </c>
       <c r="H73" s="6" t="b">
@@ -4497,7 +4392,7 @@
       <c r="J73" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="K73" s="5"/>
+      <c r="K73" s="6"/>
       <c r="L73" s="8" t="s">
         <v>19</v>
       </c>
@@ -4506,657 +4401,13 @@
       </c>
       <c r="N73" s="8"/>
       <c r="O73" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B74" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E74" s="5">
-        <v>0</v>
-      </c>
-      <c r="F74" s="5">
-        <v>0</v>
-      </c>
-      <c r="G74" s="5">
-        <v>1</v>
-      </c>
-      <c r="H74" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I74" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J74" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K74" s="5"/>
-      <c r="L74" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M74" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N74" s="8"/>
-      <c r="O74" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E75" s="5">
-        <v>1</v>
-      </c>
-      <c r="F75" s="5">
-        <v>0</v>
-      </c>
-      <c r="G75" s="5">
-        <v>1</v>
-      </c>
-      <c r="H75" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I75" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J75" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K75" s="5"/>
-      <c r="L75" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M75" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N75" s="8"/>
-      <c r="O75" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E76" s="5">
-        <v>1</v>
-      </c>
-      <c r="F76" s="5">
-        <v>1</v>
-      </c>
-      <c r="G76" s="5">
-        <v>0</v>
-      </c>
-      <c r="H76" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I76" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J76" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K76" s="5"/>
-      <c r="L76" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M76" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N76" s="8"/>
-      <c r="O76" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E77" s="5">
-        <v>1</v>
-      </c>
-      <c r="F77" s="5">
-        <v>1</v>
-      </c>
-      <c r="G77" s="5">
-        <v>1</v>
-      </c>
-      <c r="H77" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I77" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J77" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K77" s="5"/>
-      <c r="L77" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M77" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N77" s="8"/>
-      <c r="O77" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="5">
-        <v>1</v>
-      </c>
-      <c r="F78" s="5">
-        <v>0</v>
-      </c>
-      <c r="G78" s="5">
-        <v>0</v>
-      </c>
-      <c r="H78" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I78" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J78" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K78" s="5"/>
-      <c r="L78" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M78" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N78" s="8"/>
-      <c r="O78" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="16"/>
-      <c r="E79" s="6">
-        <v>0</v>
-      </c>
-      <c r="F79" s="6">
-        <v>0</v>
-      </c>
-      <c r="G79" s="6">
-        <v>1</v>
-      </c>
-      <c r="H79" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I79" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J79" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K79" s="6"/>
-      <c r="L79" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M79" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N79" s="8"/>
-      <c r="O79" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="5">
-        <v>1</v>
-      </c>
-      <c r="F80" s="5">
-        <v>0</v>
-      </c>
-      <c r="G80" s="5">
-        <v>1</v>
-      </c>
-      <c r="H80" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I80" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J80" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K80" s="5"/>
-      <c r="L80" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M80" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N80" s="8"/>
-      <c r="O80" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="5">
-        <v>1</v>
-      </c>
-      <c r="F81" s="5">
-        <v>1</v>
-      </c>
-      <c r="G81" s="5">
-        <v>0</v>
-      </c>
-      <c r="H81" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I81" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J81" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K81" s="5"/>
-      <c r="L81" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M81" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N81" s="8"/>
-      <c r="O81" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="5">
-        <v>1</v>
-      </c>
-      <c r="F82" s="5">
-        <v>1</v>
-      </c>
-      <c r="G82" s="5">
-        <v>1</v>
-      </c>
-      <c r="H82" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I82" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J82" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K82" s="5"/>
-      <c r="L82" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M82" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N82" s="8"/>
-      <c r="O82" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="16">
-        <v>25</v>
-      </c>
-      <c r="E83" s="5">
-        <v>1</v>
-      </c>
-      <c r="F83" s="5">
-        <v>0</v>
-      </c>
-      <c r="G83" s="5">
-        <v>0</v>
-      </c>
-      <c r="H83" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I83" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J83" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K83" s="5"/>
-      <c r="L83" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M83" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N83" s="8"/>
-      <c r="O83" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="16">
-        <v>25</v>
-      </c>
-      <c r="E84" s="5">
-        <v>0</v>
-      </c>
-      <c r="F84" s="5">
-        <v>0</v>
-      </c>
-      <c r="G84" s="5">
-        <v>1</v>
-      </c>
-      <c r="H84" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I84" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J84" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K84" s="5"/>
-      <c r="L84" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M84" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N84" s="8"/>
-      <c r="O84" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="16">
-        <v>25</v>
-      </c>
-      <c r="E85" s="5">
-        <v>1</v>
-      </c>
-      <c r="F85" s="5">
-        <v>0</v>
-      </c>
-      <c r="G85" s="5">
-        <v>1</v>
-      </c>
-      <c r="H85" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I85" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J85" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K85" s="5"/>
-      <c r="L85" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M85" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N85" s="8"/>
-      <c r="O85" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B86" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C86" s="5"/>
-      <c r="D86" s="16">
-        <v>25</v>
-      </c>
-      <c r="E86" s="5">
-        <v>1</v>
-      </c>
-      <c r="F86" s="5">
-        <v>1</v>
-      </c>
-      <c r="G86" s="5">
-        <v>0</v>
-      </c>
-      <c r="H86" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I86" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J86" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K86" s="5"/>
-      <c r="L86" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M86" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N86" s="8"/>
-      <c r="O86" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B87" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="16">
-        <v>25</v>
-      </c>
-      <c r="E87" s="5">
-        <v>1</v>
-      </c>
-      <c r="F87" s="5">
-        <v>1</v>
-      </c>
-      <c r="G87" s="5">
-        <v>1</v>
-      </c>
-      <c r="H87" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I87" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J87" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K87" s="5"/>
-      <c r="L87" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M87" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N87" s="8"/>
-      <c r="O87" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A88" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E88" s="6">
-        <v>1</v>
-      </c>
-      <c r="F88" s="6">
-        <v>0</v>
-      </c>
-      <c r="G88" s="6">
-        <v>0</v>
-      </c>
-      <c r="H88" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I88" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J88" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K88" s="6"/>
-      <c r="L88" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M88" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N88" s="8"/>
-      <c r="O88" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A89" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B89" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C89" s="6"/>
-      <c r="D89" s="16"/>
-      <c r="E89" s="6">
-        <v>1</v>
-      </c>
-      <c r="F89" s="6">
-        <v>0</v>
-      </c>
-      <c r="G89" s="6">
-        <v>0</v>
-      </c>
-      <c r="H89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I89" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J89" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K89" s="6"/>
-      <c r="L89" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M89" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N89" s="8"/>
-      <c r="O89" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1048566">
-      <formula1>$O$1048566:$O$1048572</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1048550">
+      <formula1>$O$1048550:$O$1048556</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tests pointed to QA Env, added search to book flows
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
@@ -607,6 +607,288 @@
   </cellStyles>
   <dxfs count="59">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -874,288 +1156,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1531,6 +1531,30 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:O23" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A1:O23"/>
   <tableColumns count="15">
+    <tableColumn id="1" name="Description" dataDxfId="34"/>
+    <tableColumn id="2" name="TripType" dataDxfId="33"/>
+    <tableColumn id="3" name="AirPortPairs" dataDxfId="32"/>
+    <tableColumn id="4" name="TravelDates" dataDxfId="31"/>
+    <tableColumn id="5" name="Adults" dataDxfId="30"/>
+    <tableColumn id="6" name="Infants" dataDxfId="29"/>
+    <tableColumn id="7" name="Children" dataDxfId="28"/>
+    <tableColumn id="8" name="IncludeNearByAirPorts" dataDxfId="27"/>
+    <tableColumn id="9" name="CabinType" dataDxfId="26"/>
+    <tableColumn id="10" name="NonStopFlight" dataDxfId="25"/>
+    <tableColumn id="11" name="AirLines" dataDxfId="24"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="23"/>
+    <tableColumn id="14" name="SpecialFilterName" dataDxfId="22"/>
+    <tableColumn id="15" name="SpecialFilterValues" dataDxfId="21"/>
+    <tableColumn id="12" name="UserType" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table234" displayName="Table234" ref="A1:O73" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:O73"/>
+  <tableColumns count="15">
     <tableColumn id="1" name="Description" dataDxfId="14"/>
     <tableColumn id="2" name="TripType" dataDxfId="13"/>
     <tableColumn id="3" name="AirPortPairs" dataDxfId="12"/>
@@ -1546,30 +1570,6 @@
     <tableColumn id="14" name="SpecialFilterName" dataDxfId="2"/>
     <tableColumn id="15" name="SpecialFilterValues" dataDxfId="1"/>
     <tableColumn id="12" name="UserType" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table234" displayName="Table234" ref="A1:O73" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
-  <autoFilter ref="A1:O73"/>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="29"/>
-    <tableColumn id="2" name="TripType" dataDxfId="28"/>
-    <tableColumn id="3" name="AirPortPairs" dataDxfId="27"/>
-    <tableColumn id="4" name="TravelDates" dataDxfId="26"/>
-    <tableColumn id="5" name="Adults" dataDxfId="25"/>
-    <tableColumn id="6" name="Infants" dataDxfId="24"/>
-    <tableColumn id="7" name="Children" dataDxfId="23"/>
-    <tableColumn id="8" name="IncludeNearByAirPorts" dataDxfId="22"/>
-    <tableColumn id="9" name="CabinType" dataDxfId="21"/>
-    <tableColumn id="10" name="NonStopFlight" dataDxfId="20"/>
-    <tableColumn id="11" name="AirLines" dataDxfId="19"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="18"/>
-    <tableColumn id="14" name="SpecialFilterName" dataDxfId="17"/>
-    <tableColumn id="15" name="SpecialFilterValues" dataDxfId="16"/>
-    <tableColumn id="12" name="UserType" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5118,8 +5118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5189,26 +5189,26 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="39" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>29</v>
+      <c r="A2" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="33">
+        <v>25</v>
       </c>
       <c r="E2" s="23">
         <v>1</v>
       </c>
       <c r="F2" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="21" t="b">
         <v>0</v>
@@ -5235,25 +5235,25 @@
     </row>
     <row r="3" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>104</v>
+        <v>29</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>17</v>
       </c>
       <c r="E3" s="23">
         <v>1</v>
       </c>
       <c r="F3" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="21" t="b">
         <v>0</v>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="4" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>35</v>
@@ -5291,14 +5291,14 @@
       <c r="D4" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="21">
-        <v>1</v>
-      </c>
-      <c r="F4" s="21">
-        <v>0</v>
-      </c>
-      <c r="G4" s="21">
-        <v>1</v>
+      <c r="E4" s="23">
+        <v>1</v>
+      </c>
+      <c r="F4" s="23">
+        <v>0</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0</v>
       </c>
       <c r="H4" s="21" t="b">
         <v>0</v>
@@ -5309,7 +5309,7 @@
       <c r="J4" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="K4" s="21"/>
+      <c r="K4" s="23"/>
       <c r="L4" s="8" t="s">
         <v>33</v>
       </c>
@@ -5324,10 +5324,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="39" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="23" t="s">
@@ -5336,14 +5336,14 @@
       <c r="D5" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="23">
-        <v>1</v>
-      </c>
-      <c r="F5" s="23">
-        <v>1</v>
-      </c>
-      <c r="G5" s="23">
-        <v>0</v>
+      <c r="E5" s="21">
+        <v>1</v>
+      </c>
+      <c r="F5" s="21">
+        <v>0</v>
+      </c>
+      <c r="G5" s="21">
+        <v>1</v>
       </c>
       <c r="H5" s="21" t="b">
         <v>0</v>
@@ -5354,7 +5354,7 @@
       <c r="J5" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="K5" s="23"/>
+      <c r="K5" s="21"/>
       <c r="L5" s="8" t="s">
         <v>33</v>
       </c>
@@ -5370,7 +5370,7 @@
     </row>
     <row r="6" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>35</v>
@@ -5388,7 +5388,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="21" t="b">
         <v>0</v>
@@ -5415,25 +5415,25 @@
     </row>
     <row r="7" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="33">
-        <v>25</v>
+        <v>103</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>104</v>
       </c>
       <c r="E7" s="23">
         <v>1</v>
       </c>
       <c r="F7" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="21" t="b">
         <v>0</v>
@@ -6212,7 +6212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added a structure for validations and exceptions
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AirLoginRoviaBucks" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="111">
   <si>
     <t>Description</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>Guest</t>
+  </si>
+  <si>
+    <t>LAS-LAX|LAX-DFW|DFW-MIA|MIA-SIN|SIN-DEL</t>
+  </si>
+  <si>
+    <t>53|64|71|80|90</t>
   </si>
 </sst>
 </file>
@@ -1552,8 +1558,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table234" displayName="Table234" ref="A1:O73" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="A1:O73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table234" displayName="Table234" ref="A1:O19" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:O19"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Description" dataDxfId="14"/>
     <tableColumn id="2" name="TripType" dataDxfId="13"/>
@@ -5118,8 +5124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5189,17 +5195,17 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="39" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>32</v>
+      <c r="A2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>35</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="33">
-        <v>25</v>
+        <v>109</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>110</v>
       </c>
       <c r="E2" s="23">
         <v>1</v>
@@ -6210,10 +6216,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7092,2360 +7098,6 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="16">
-        <v>25</v>
-      </c>
-      <c r="E20" s="5">
-        <v>1</v>
-      </c>
-      <c r="F20" s="5">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5">
-        <v>0</v>
-      </c>
-      <c r="H20" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N20" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="16">
-        <v>25</v>
-      </c>
-      <c r="E21" s="5">
-        <v>1</v>
-      </c>
-      <c r="F21" s="5">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
-        <v>1</v>
-      </c>
-      <c r="H21" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="16">
-        <v>25</v>
-      </c>
-      <c r="E22" s="6">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6">
-        <v>1</v>
-      </c>
-      <c r="G22" s="6">
-        <v>0</v>
-      </c>
-      <c r="H22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="16">
-        <v>25</v>
-      </c>
-      <c r="E23" s="5">
-        <v>1</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1</v>
-      </c>
-      <c r="G23" s="5">
-        <v>1</v>
-      </c>
-      <c r="H23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N23" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O23" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="5">
-        <v>1</v>
-      </c>
-      <c r="F24" s="5">
-        <v>0</v>
-      </c>
-      <c r="G24" s="5">
-        <v>0</v>
-      </c>
-      <c r="H24" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L24" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N24" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O24" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="5">
-        <v>1</v>
-      </c>
-      <c r="F25" s="5">
-        <v>0</v>
-      </c>
-      <c r="G25" s="5">
-        <v>1</v>
-      </c>
-      <c r="H25" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O25" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="5">
-        <v>1</v>
-      </c>
-      <c r="F26" s="5">
-        <v>1</v>
-      </c>
-      <c r="G26" s="5">
-        <v>0</v>
-      </c>
-      <c r="H26" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N26" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O26" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="5">
-        <v>1</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1</v>
-      </c>
-      <c r="G27" s="5">
-        <v>1</v>
-      </c>
-      <c r="H27" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J27" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N27" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O27" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" s="5">
-        <v>1</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0</v>
-      </c>
-      <c r="G28" s="5">
-        <v>0</v>
-      </c>
-      <c r="H28" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J28" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N28" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O28" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" s="5">
-        <v>1</v>
-      </c>
-      <c r="F29" s="5">
-        <v>0</v>
-      </c>
-      <c r="G29" s="5">
-        <v>1</v>
-      </c>
-      <c r="H29" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J29" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L29" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M29" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N29" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O29" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="5">
-        <v>1</v>
-      </c>
-      <c r="F30" s="5">
-        <v>1</v>
-      </c>
-      <c r="G30" s="5">
-        <v>0</v>
-      </c>
-      <c r="H30" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J30" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N30" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O30" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" s="5">
-        <v>1</v>
-      </c>
-      <c r="F31" s="5">
-        <v>1</v>
-      </c>
-      <c r="G31" s="5">
-        <v>1</v>
-      </c>
-      <c r="H31" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J31" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N31" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O31" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="16">
-        <v>25</v>
-      </c>
-      <c r="E32" s="5">
-        <v>1</v>
-      </c>
-      <c r="F32" s="5">
-        <v>0</v>
-      </c>
-      <c r="G32" s="5">
-        <v>0</v>
-      </c>
-      <c r="H32" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K32" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M32" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N32" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O32" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" s="16">
-        <v>25</v>
-      </c>
-      <c r="E33" s="5">
-        <v>1</v>
-      </c>
-      <c r="F33" s="5">
-        <v>0</v>
-      </c>
-      <c r="G33" s="5">
-        <v>1</v>
-      </c>
-      <c r="H33" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M33" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N33" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O33" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="16">
-        <v>25</v>
-      </c>
-      <c r="E34" s="5">
-        <v>1</v>
-      </c>
-      <c r="F34" s="5">
-        <v>1</v>
-      </c>
-      <c r="G34" s="5">
-        <v>0</v>
-      </c>
-      <c r="H34" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L34" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M34" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N34" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O34" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D35" s="16">
-        <v>25</v>
-      </c>
-      <c r="E35" s="5">
-        <v>1</v>
-      </c>
-      <c r="F35" s="5">
-        <v>1</v>
-      </c>
-      <c r="G35" s="5">
-        <v>1</v>
-      </c>
-      <c r="H35" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J35" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N35" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O35" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="6">
-        <v>1</v>
-      </c>
-      <c r="F36" s="6">
-        <v>0</v>
-      </c>
-      <c r="G36" s="6">
-        <v>0</v>
-      </c>
-      <c r="H36" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J36" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L36" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M36" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N36" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" s="5">
-        <v>1</v>
-      </c>
-      <c r="F37" s="5">
-        <v>0</v>
-      </c>
-      <c r="G37" s="5">
-        <v>0</v>
-      </c>
-      <c r="H37" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J37" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N37" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O37" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" s="16">
-        <v>25</v>
-      </c>
-      <c r="E38" s="5">
-        <v>1</v>
-      </c>
-      <c r="F38" s="5">
-        <v>0</v>
-      </c>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
-      <c r="H38" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J38" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K38" s="5"/>
-      <c r="L38" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M38" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N38" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O38" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" s="16">
-        <v>25</v>
-      </c>
-      <c r="E39" s="5">
-        <v>1</v>
-      </c>
-      <c r="F39" s="5">
-        <v>0</v>
-      </c>
-      <c r="G39" s="5">
-        <v>1</v>
-      </c>
-      <c r="H39" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J39" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K39" s="5"/>
-      <c r="L39" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M39" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N39" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O39" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="16">
-        <v>25</v>
-      </c>
-      <c r="E40" s="5">
-        <v>1</v>
-      </c>
-      <c r="F40" s="5">
-        <v>1</v>
-      </c>
-      <c r="G40" s="5">
-        <v>0</v>
-      </c>
-      <c r="H40" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J40" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K40" s="5"/>
-      <c r="L40" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M40" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N40" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O40" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D41" s="16">
-        <v>25</v>
-      </c>
-      <c r="E41" s="5">
-        <v>1</v>
-      </c>
-      <c r="F41" s="5">
-        <v>1</v>
-      </c>
-      <c r="G41" s="5">
-        <v>1</v>
-      </c>
-      <c r="H41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J41" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K41" s="5"/>
-      <c r="L41" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M41" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N41" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O41" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="5">
-        <v>1</v>
-      </c>
-      <c r="F42" s="5">
-        <v>0</v>
-      </c>
-      <c r="G42" s="5">
-        <v>0</v>
-      </c>
-      <c r="H42" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J42" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K42" s="5"/>
-      <c r="L42" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M42" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N42" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O42" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="5">
-        <v>1</v>
-      </c>
-      <c r="F43" s="5">
-        <v>0</v>
-      </c>
-      <c r="G43" s="5">
-        <v>1</v>
-      </c>
-      <c r="H43" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J43" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K43" s="5"/>
-      <c r="L43" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M43" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N43" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O43" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" s="5">
-        <v>1</v>
-      </c>
-      <c r="F44" s="5">
-        <v>1</v>
-      </c>
-      <c r="G44" s="5">
-        <v>0</v>
-      </c>
-      <c r="H44" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J44" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K44" s="5"/>
-      <c r="L44" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M44" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N44" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O44" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" s="5">
-        <v>1</v>
-      </c>
-      <c r="F45" s="5">
-        <v>1</v>
-      </c>
-      <c r="G45" s="5">
-        <v>1</v>
-      </c>
-      <c r="H45" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J45" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K45" s="5"/>
-      <c r="L45" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M45" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N45" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O45" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="5">
-        <v>1</v>
-      </c>
-      <c r="F46" s="5">
-        <v>0</v>
-      </c>
-      <c r="G46" s="5">
-        <v>0</v>
-      </c>
-      <c r="H46" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I46" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J46" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K46" s="5"/>
-      <c r="L46" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M46" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N46" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O46" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="5">
-        <v>1</v>
-      </c>
-      <c r="F47" s="5">
-        <v>0</v>
-      </c>
-      <c r="G47" s="5">
-        <v>1</v>
-      </c>
-      <c r="H47" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J47" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K47" s="5"/>
-      <c r="L47" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M47" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N47" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O47" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="5">
-        <v>1</v>
-      </c>
-      <c r="F48" s="5">
-        <v>1</v>
-      </c>
-      <c r="G48" s="5">
-        <v>0</v>
-      </c>
-      <c r="H48" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J48" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K48" s="5"/>
-      <c r="L48" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M48" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N48" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O48" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="5">
-        <v>1</v>
-      </c>
-      <c r="F49" s="5">
-        <v>1</v>
-      </c>
-      <c r="G49" s="5">
-        <v>1</v>
-      </c>
-      <c r="H49" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J49" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K49" s="5"/>
-      <c r="L49" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M49" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N49" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O49" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="16">
-        <v>25</v>
-      </c>
-      <c r="E50" s="6">
-        <v>1</v>
-      </c>
-      <c r="F50" s="6">
-        <v>0</v>
-      </c>
-      <c r="G50" s="6">
-        <v>0</v>
-      </c>
-      <c r="H50" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J50" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K50" s="6"/>
-      <c r="L50" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M50" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N50" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O50" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="16">
-        <v>25</v>
-      </c>
-      <c r="E51" s="5">
-        <v>1</v>
-      </c>
-      <c r="F51" s="5">
-        <v>0</v>
-      </c>
-      <c r="G51" s="5">
-        <v>1</v>
-      </c>
-      <c r="H51" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J51" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K51" s="5"/>
-      <c r="L51" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M51" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N51" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O51" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="16">
-        <v>25</v>
-      </c>
-      <c r="E52" s="5">
-        <v>1</v>
-      </c>
-      <c r="F52" s="5">
-        <v>1</v>
-      </c>
-      <c r="G52" s="5">
-        <v>0</v>
-      </c>
-      <c r="H52" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J52" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K52" s="5"/>
-      <c r="L52" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M52" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N52" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O52" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="16">
-        <v>25</v>
-      </c>
-      <c r="E53" s="5">
-        <v>1</v>
-      </c>
-      <c r="F53" s="5">
-        <v>1</v>
-      </c>
-      <c r="G53" s="5">
-        <v>1</v>
-      </c>
-      <c r="H53" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J53" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K53" s="5"/>
-      <c r="L53" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M53" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N53" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O53" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E54" s="5">
-        <v>1</v>
-      </c>
-      <c r="F54" s="5">
-        <v>0</v>
-      </c>
-      <c r="G54" s="5">
-        <v>0</v>
-      </c>
-      <c r="H54" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I54" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J54" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K54" s="5"/>
-      <c r="L54" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M54" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N54" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O54" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="5">
-        <v>1</v>
-      </c>
-      <c r="F55" s="5">
-        <v>0</v>
-      </c>
-      <c r="G55" s="5">
-        <v>0</v>
-      </c>
-      <c r="H55" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I55" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J55" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K55" s="5"/>
-      <c r="L55" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M55" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N55" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O55" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="16">
-        <v>25</v>
-      </c>
-      <c r="E56" s="5">
-        <v>1</v>
-      </c>
-      <c r="F56" s="5">
-        <v>0</v>
-      </c>
-      <c r="G56" s="5">
-        <v>0</v>
-      </c>
-      <c r="H56" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I56" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J56" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K56" s="5"/>
-      <c r="L56" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M56" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N56" s="8"/>
-      <c r="O56" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="16">
-        <v>25</v>
-      </c>
-      <c r="E57" s="5">
-        <v>1</v>
-      </c>
-      <c r="F57" s="5">
-        <v>0</v>
-      </c>
-      <c r="G57" s="5">
-        <v>1</v>
-      </c>
-      <c r="H57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J57" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K57" s="5"/>
-      <c r="L57" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M57" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N57" s="8"/>
-      <c r="O57" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="16">
-        <v>25</v>
-      </c>
-      <c r="E58" s="6">
-        <v>1</v>
-      </c>
-      <c r="F58" s="6">
-        <v>1</v>
-      </c>
-      <c r="G58" s="6">
-        <v>0</v>
-      </c>
-      <c r="H58" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I58" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J58" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K58" s="6"/>
-      <c r="L58" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M58" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N58" s="8"/>
-      <c r="O58" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="16">
-        <v>25</v>
-      </c>
-      <c r="E59" s="5">
-        <v>1</v>
-      </c>
-      <c r="F59" s="5">
-        <v>1</v>
-      </c>
-      <c r="G59" s="5">
-        <v>1</v>
-      </c>
-      <c r="H59" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I59" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J59" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K59" s="5"/>
-      <c r="L59" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M59" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N59" s="8"/>
-      <c r="O59" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60" s="5">
-        <v>1</v>
-      </c>
-      <c r="F60" s="5">
-        <v>0</v>
-      </c>
-      <c r="G60" s="5">
-        <v>0</v>
-      </c>
-      <c r="H60" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J60" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K60" s="5"/>
-      <c r="L60" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M60" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N60" s="8"/>
-      <c r="O60" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E61" s="5">
-        <v>1</v>
-      </c>
-      <c r="F61" s="5">
-        <v>0</v>
-      </c>
-      <c r="G61" s="5">
-        <v>1</v>
-      </c>
-      <c r="H61" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I61" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J61" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K61" s="5"/>
-      <c r="L61" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M61" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N61" s="8"/>
-      <c r="O61" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E62" s="5">
-        <v>1</v>
-      </c>
-      <c r="F62" s="5">
-        <v>1</v>
-      </c>
-      <c r="G62" s="5">
-        <v>0</v>
-      </c>
-      <c r="H62" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I62" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J62" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K62" s="5"/>
-      <c r="L62" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M62" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N62" s="8"/>
-      <c r="O62" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E63" s="5">
-        <v>1</v>
-      </c>
-      <c r="F63" s="5">
-        <v>1</v>
-      </c>
-      <c r="G63" s="5">
-        <v>1</v>
-      </c>
-      <c r="H63" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I63" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J63" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K63" s="5"/>
-      <c r="L63" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M63" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N63" s="8"/>
-      <c r="O63" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="5">
-        <v>1</v>
-      </c>
-      <c r="F64" s="5">
-        <v>0</v>
-      </c>
-      <c r="G64" s="5">
-        <v>0</v>
-      </c>
-      <c r="H64" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I64" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J64" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K64" s="5"/>
-      <c r="L64" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M64" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N64" s="8"/>
-      <c r="O64" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="5">
-        <v>1</v>
-      </c>
-      <c r="F65" s="5">
-        <v>0</v>
-      </c>
-      <c r="G65" s="5">
-        <v>1</v>
-      </c>
-      <c r="H65" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I65" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J65" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K65" s="5"/>
-      <c r="L65" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M65" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N65" s="8"/>
-      <c r="O65" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="5">
-        <v>1</v>
-      </c>
-      <c r="F66" s="5">
-        <v>1</v>
-      </c>
-      <c r="G66" s="5">
-        <v>0</v>
-      </c>
-      <c r="H66" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I66" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J66" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K66" s="5"/>
-      <c r="L66" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M66" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N66" s="8"/>
-      <c r="O66" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="5">
-        <v>1</v>
-      </c>
-      <c r="F67" s="5">
-        <v>1</v>
-      </c>
-      <c r="G67" s="5">
-        <v>1</v>
-      </c>
-      <c r="H67" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I67" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J67" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K67" s="5"/>
-      <c r="L67" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M67" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N67" s="8"/>
-      <c r="O67" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="16">
-        <v>25</v>
-      </c>
-      <c r="E68" s="5">
-        <v>1</v>
-      </c>
-      <c r="F68" s="5">
-        <v>0</v>
-      </c>
-      <c r="G68" s="5">
-        <v>0</v>
-      </c>
-      <c r="H68" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I68" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J68" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K68" s="5"/>
-      <c r="L68" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M68" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N68" s="8"/>
-      <c r="O68" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C69" s="5"/>
-      <c r="D69" s="16">
-        <v>25</v>
-      </c>
-      <c r="E69" s="5">
-        <v>1</v>
-      </c>
-      <c r="F69" s="5">
-        <v>0</v>
-      </c>
-      <c r="G69" s="5">
-        <v>1</v>
-      </c>
-      <c r="H69" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I69" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J69" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K69" s="5"/>
-      <c r="L69" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M69" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N69" s="8"/>
-      <c r="O69" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C70" s="5"/>
-      <c r="D70" s="16">
-        <v>25</v>
-      </c>
-      <c r="E70" s="5">
-        <v>1</v>
-      </c>
-      <c r="F70" s="5">
-        <v>1</v>
-      </c>
-      <c r="G70" s="5">
-        <v>0</v>
-      </c>
-      <c r="H70" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I70" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J70" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K70" s="5"/>
-      <c r="L70" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M70" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N70" s="8"/>
-      <c r="O70" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="16">
-        <v>25</v>
-      </c>
-      <c r="E71" s="5">
-        <v>1</v>
-      </c>
-      <c r="F71" s="5">
-        <v>1</v>
-      </c>
-      <c r="G71" s="5">
-        <v>1</v>
-      </c>
-      <c r="H71" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I71" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J71" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K71" s="5"/>
-      <c r="L71" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M71" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N71" s="8"/>
-      <c r="O71" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E72" s="6">
-        <v>1</v>
-      </c>
-      <c r="F72" s="6">
-        <v>0</v>
-      </c>
-      <c r="G72" s="6">
-        <v>0</v>
-      </c>
-      <c r="H72" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I72" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J72" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K72" s="6"/>
-      <c r="L72" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M72" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N72" s="8"/>
-      <c r="O72" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="6">
-        <v>1</v>
-      </c>
-      <c r="F73" s="6">
-        <v>0</v>
-      </c>
-      <c r="G73" s="6">
-        <v>0</v>
-      </c>
-      <c r="H73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I73" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J73" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K73" s="6"/>
-      <c r="L73" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M73" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N73" s="8"/>
-      <c r="O73" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
reading and setting post search filters values from sheet
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AirLoginRoviaBucks" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="130">
   <si>
     <t>Description</t>
   </si>
@@ -355,6 +355,57 @@
   </si>
   <si>
     <t>Search|AddToCart</t>
+  </si>
+  <si>
+    <t>PostFilters</t>
+  </si>
+  <si>
+    <t>PostFiltersValues</t>
+  </si>
+  <si>
+    <t>Price|Stop|Duration|Cabin|Airlines</t>
+  </si>
+  <si>
+    <t>20-30|one|10|economy,business|NK,AA</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>30-20</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Search|SETFILTERS</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>one-plus</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Cabin</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>economy</t>
+  </si>
+  <si>
+    <t>Airlines</t>
+  </si>
+  <si>
+    <t>NK,AA</t>
   </si>
 </sst>
 </file>
@@ -617,7 +668,250 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="64">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -640,18 +934,320 @@
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -698,6 +1294,304 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -718,398 +1612,7 @@
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1123,436 +1626,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1632,36 +1705,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:P73" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:P73" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="A1:P73"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="Description" dataDxfId="56"/>
-    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="0"/>
-    <tableColumn id="2" name="TripType" dataDxfId="55"/>
-    <tableColumn id="3" name="AirPortPairs" dataDxfId="54"/>
-    <tableColumn id="4" name="TravelDates" dataDxfId="53"/>
-    <tableColumn id="5" name="Adults" dataDxfId="52"/>
-    <tableColumn id="6" name="Infants" dataDxfId="51"/>
-    <tableColumn id="7" name="Children" dataDxfId="50"/>
-    <tableColumn id="8" name="IncludeNearByAirPorts" dataDxfId="49"/>
-    <tableColumn id="9" name="CabinType" dataDxfId="48"/>
-    <tableColumn id="10" name="NonStopFlight" dataDxfId="47"/>
-    <tableColumn id="11" name="AirLines" dataDxfId="46"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="45"/>
-    <tableColumn id="14" name="SpecialFilterName" dataDxfId="44"/>
-    <tableColumn id="15" name="SpecialFilterValues" dataDxfId="43"/>
-    <tableColumn id="12" name="UserType" dataDxfId="42"/>
+    <tableColumn id="1" name="Description" dataDxfId="58"/>
+    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="57"/>
+    <tableColumn id="2" name="TripType" dataDxfId="56"/>
+    <tableColumn id="3" name="AirPortPairs" dataDxfId="55"/>
+    <tableColumn id="4" name="TravelDates" dataDxfId="54"/>
+    <tableColumn id="5" name="Adults" dataDxfId="53"/>
+    <tableColumn id="6" name="Infants" dataDxfId="52"/>
+    <tableColumn id="7" name="Children" dataDxfId="51"/>
+    <tableColumn id="8" name="IncludeNearByAirPorts" dataDxfId="50"/>
+    <tableColumn id="9" name="CabinType" dataDxfId="49"/>
+    <tableColumn id="10" name="NonStopFlight" dataDxfId="48"/>
+    <tableColumn id="11" name="AirLines" dataDxfId="47"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="46"/>
+    <tableColumn id="14" name="SpecialFilterName" dataDxfId="45"/>
+    <tableColumn id="15" name="SpecialFilterValues" dataDxfId="44"/>
+    <tableColumn id="12" name="UserType" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:P23" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:P23" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40" totalsRowBorderDxfId="39">
   <autoFilter ref="A1:P23"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="Description" dataDxfId="37"/>
-    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="1"/>
+    <tableColumn id="1" name="Description" dataDxfId="38"/>
+    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="37"/>
     <tableColumn id="2" name="TripType" dataDxfId="36"/>
     <tableColumn id="3" name="AirPortPairs" dataDxfId="35"/>
     <tableColumn id="4" name="TravelDates" dataDxfId="34"/>
@@ -1682,25 +1755,27 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table234" displayName="Table234" ref="A1:P19" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
-  <autoFilter ref="A1:P19"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table234" displayName="Table234" ref="A1:R19" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="A1:R19"/>
+  <tableColumns count="18">
     <tableColumn id="1" name="Description" dataDxfId="17"/>
-    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="2"/>
-    <tableColumn id="2" name="TripType" dataDxfId="16"/>
-    <tableColumn id="3" name="AirPortPairs" dataDxfId="15"/>
-    <tableColumn id="4" name="TravelDates" dataDxfId="14"/>
-    <tableColumn id="5" name="Adults" dataDxfId="13"/>
-    <tableColumn id="6" name="Infants" dataDxfId="12"/>
-    <tableColumn id="7" name="Children" dataDxfId="11"/>
-    <tableColumn id="8" name="IncludeNearByAirPorts" dataDxfId="10"/>
-    <tableColumn id="9" name="CabinType" dataDxfId="9"/>
-    <tableColumn id="10" name="NonStopFlight" dataDxfId="8"/>
-    <tableColumn id="11" name="AirLines" dataDxfId="7"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="6"/>
-    <tableColumn id="14" name="SpecialFilterName" dataDxfId="5"/>
-    <tableColumn id="15" name="SpecialFilterValues" dataDxfId="4"/>
-    <tableColumn id="12" name="UserType" dataDxfId="3"/>
+    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="16"/>
+    <tableColumn id="2" name="TripType" dataDxfId="15"/>
+    <tableColumn id="3" name="AirPortPairs" dataDxfId="14"/>
+    <tableColumn id="4" name="TravelDates" dataDxfId="13"/>
+    <tableColumn id="5" name="Adults" dataDxfId="12"/>
+    <tableColumn id="6" name="Infants" dataDxfId="11"/>
+    <tableColumn id="7" name="Children" dataDxfId="10"/>
+    <tableColumn id="8" name="IncludeNearByAirPorts" dataDxfId="9"/>
+    <tableColumn id="9" name="CabinType" dataDxfId="8"/>
+    <tableColumn id="10" name="NonStopFlight" dataDxfId="7"/>
+    <tableColumn id="11" name="AirLines" dataDxfId="6"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="5"/>
+    <tableColumn id="14" name="SpecialFilterName" dataDxfId="4"/>
+    <tableColumn id="15" name="SpecialFilterValues" dataDxfId="3"/>
+    <tableColumn id="12" name="UserType" dataDxfId="2"/>
+    <tableColumn id="17" name="PostFilters" dataDxfId="1"/>
+    <tableColumn id="18" name="PostFiltersValues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1995,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="D73" sqref="D73"/>
@@ -5468,8 +5543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6629,15 +6704,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
@@ -6652,9 +6728,11 @@
     <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -6703,13 +6781,19 @@
       <c r="P1" s="28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q1" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>32</v>
@@ -6751,13 +6835,19 @@
       <c r="P2" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>32</v>
@@ -6799,13 +6889,19 @@
       <c r="P3" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>32</v>
@@ -6847,13 +6943,19 @@
       <c r="P4" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q4" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="R4" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>32</v>
@@ -6895,13 +6997,19 @@
       <c r="P5" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q5" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>15</v>
@@ -6943,13 +7051,19 @@
       <c r="P6" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q6" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>15</v>
@@ -6991,13 +7105,19 @@
       <c r="P7" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q7" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>15</v>
@@ -7039,13 +7159,19 @@
       <c r="P8" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q8" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>15</v>
@@ -7087,13 +7213,19 @@
       <c r="P9" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q9" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>35</v>
@@ -7135,13 +7267,15 @@
       <c r="P10" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+    </row>
+    <row r="11" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>35</v>
@@ -7183,13 +7317,15 @@
       <c r="P11" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+    </row>
+    <row r="12" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>35</v>
@@ -7231,13 +7367,15 @@
       <c r="P12" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+    </row>
+    <row r="13" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>35</v>
@@ -7279,13 +7417,15 @@
       <c r="P13" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+    </row>
+    <row r="14" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>32</v>
@@ -7327,13 +7467,15 @@
       <c r="P14" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+    </row>
+    <row r="15" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>32</v>
@@ -7375,13 +7517,15 @@
       <c r="P15" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+    </row>
+    <row r="16" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>32</v>
@@ -7423,13 +7567,15 @@
       <c r="P16" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+    </row>
+    <row r="17" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>32</v>
@@ -7471,13 +7617,15 @@
       <c r="P17" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+    </row>
+    <row r="18" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>15</v>
@@ -7519,13 +7667,15 @@
       <c r="P18" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+    </row>
+    <row r="19" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>35</v>
@@ -7567,6 +7717,8 @@
       <c r="P19" s="9" t="s">
         <v>108</v>
       </c>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added a test for car search
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AirLoginRoviaBucks" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="130">
   <si>
     <t>Description</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>AA/NK</t>
+  </si>
+  <si>
+    <t>Search</t>
   </si>
 </sst>
 </file>
@@ -634,74 +637,6 @@
   </cellStyles>
   <dxfs count="64">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -798,6 +733,24 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -812,6 +765,22 @@
         <bottom/>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1124,6 +1093,24 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1138,6 +1125,22 @@
         <bottom/>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1754,41 +1757,41 @@
     <tableColumn id="5" name="Adults" dataDxfId="32"/>
     <tableColumn id="6" name="Infants" dataDxfId="31"/>
     <tableColumn id="7" name="Children" dataDxfId="30"/>
-    <tableColumn id="8" name="IncludeNearByAirPorts" dataDxfId="1"/>
-    <tableColumn id="9" name="CabinType" dataDxfId="29"/>
-    <tableColumn id="10" name="NonStopFlight" dataDxfId="0"/>
-    <tableColumn id="11" name="AirLines" dataDxfId="28"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="27"/>
-    <tableColumn id="15" name="Supplier" dataDxfId="26"/>
-    <tableColumn id="12" name="UserType" dataDxfId="25"/>
-    <tableColumn id="14" name="PostFilters" dataDxfId="24"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="23"/>
+    <tableColumn id="8" name="IncludeNearByAirPorts" dataDxfId="29"/>
+    <tableColumn id="9" name="CabinType" dataDxfId="28"/>
+    <tableColumn id="10" name="NonStopFlight" dataDxfId="27"/>
+    <tableColumn id="11" name="AirLines" dataDxfId="26"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="25"/>
+    <tableColumn id="15" name="Supplier" dataDxfId="24"/>
+    <tableColumn id="12" name="UserType" dataDxfId="23"/>
+    <tableColumn id="14" name="PostFilters" dataDxfId="22"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table234" displayName="Table234" ref="A1:Q73" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
-  <autoFilter ref="A1:Q73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table234" displayName="Table234" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="18"/>
-    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="17"/>
-    <tableColumn id="2" name="TripType" dataDxfId="16"/>
-    <tableColumn id="3" name="AirPortPairs" dataDxfId="15"/>
-    <tableColumn id="4" name="TravelDates" dataDxfId="14"/>
-    <tableColumn id="5" name="Adults" dataDxfId="13"/>
-    <tableColumn id="6" name="Infants" dataDxfId="12"/>
-    <tableColumn id="7" name="Children" dataDxfId="11"/>
-    <tableColumn id="8" name="IncludeNearByAirPorts" dataDxfId="3"/>
-    <tableColumn id="9" name="CabinType" dataDxfId="10"/>
-    <tableColumn id="10" name="NonStopFlight" dataDxfId="2"/>
-    <tableColumn id="11" name="AirLines" dataDxfId="9"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="8"/>
-    <tableColumn id="15" name="Supplier" dataDxfId="7"/>
-    <tableColumn id="12" name="UserType" dataDxfId="6"/>
-    <tableColumn id="14" name="PostFilters" dataDxfId="5"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="4"/>
+    <tableColumn id="1" name="Description" dataDxfId="16"/>
+    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="15"/>
+    <tableColumn id="2" name="TripType" dataDxfId="14"/>
+    <tableColumn id="3" name="AirPortPairs" dataDxfId="13"/>
+    <tableColumn id="4" name="TravelDates" dataDxfId="12"/>
+    <tableColumn id="5" name="Adults" dataDxfId="11"/>
+    <tableColumn id="6" name="Infants" dataDxfId="10"/>
+    <tableColumn id="7" name="Children" dataDxfId="9"/>
+    <tableColumn id="8" name="IncludeNearByAirPorts" dataDxfId="8"/>
+    <tableColumn id="9" name="CabinType" dataDxfId="7"/>
+    <tableColumn id="10" name="NonStopFlight" dataDxfId="6"/>
+    <tableColumn id="11" name="AirLines" dataDxfId="5"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="4"/>
+    <tableColumn id="15" name="Supplier" dataDxfId="3"/>
+    <tableColumn id="12" name="UserType" dataDxfId="2"/>
+    <tableColumn id="14" name="PostFilters" dataDxfId="1"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5577,7 +5580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
@@ -5995,7 +5998,7 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17" ht="51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>113</v>
       </c>
@@ -6042,7 +6045,7 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -9060,10 +9063,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9144,7 +9147,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>28</v>
@@ -9185,3355 +9188,6 @@
       </c>
       <c r="P2" s="23"/>
       <c r="Q2" s="23"/>
-    </row>
-    <row r="3" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="16">
-        <v>25</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
-      <c r="G3" s="10">
-        <v>0</v>
-      </c>
-      <c r="H3" s="10">
-        <v>1</v>
-      </c>
-      <c r="I3" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="16">
-        <v>25</v>
-      </c>
-      <c r="F4" s="10">
-        <v>1</v>
-      </c>
-      <c r="G4" s="10">
-        <v>1</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0</v>
-      </c>
-      <c r="I4" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-    </row>
-    <row r="5" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="16">
-        <v>25</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="10">
-        <v>1</v>
-      </c>
-      <c r="G6" s="10">
-        <v>0</v>
-      </c>
-      <c r="H6" s="10">
-        <v>0</v>
-      </c>
-      <c r="I6" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="10">
-        <v>1</v>
-      </c>
-      <c r="G7" s="10">
-        <v>0</v>
-      </c>
-      <c r="H7" s="10">
-        <v>1</v>
-      </c>
-      <c r="I7" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-    </row>
-    <row r="9" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-      <c r="I9" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-    </row>
-    <row r="11" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6">
-        <v>1</v>
-      </c>
-      <c r="I11" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-    </row>
-    <row r="12" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-    </row>
-    <row r="13" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1</v>
-      </c>
-      <c r="I13" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-    </row>
-    <row r="14" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="16">
-        <v>25</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1</v>
-      </c>
-      <c r="G14" s="5">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0</v>
-      </c>
-      <c r="I14" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" s="5"/>
-      <c r="M14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-    </row>
-    <row r="15" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="16">
-        <v>25</v>
-      </c>
-      <c r="F15" s="5">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
-        <v>1</v>
-      </c>
-      <c r="I15" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" s="5"/>
-      <c r="M15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="16">
-        <v>25</v>
-      </c>
-      <c r="F16" s="5">
-        <v>1</v>
-      </c>
-      <c r="G16" s="5">
-        <v>1</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0</v>
-      </c>
-      <c r="I16" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" s="5"/>
-      <c r="M16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="16">
-        <v>25</v>
-      </c>
-      <c r="F17" s="6">
-        <v>1</v>
-      </c>
-      <c r="G17" s="6">
-        <v>1</v>
-      </c>
-      <c r="H17" s="6">
-        <v>1</v>
-      </c>
-      <c r="I17" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="5">
-        <v>1</v>
-      </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" s="5"/>
-      <c r="M18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-    </row>
-    <row r="19" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-      <c r="G19" s="5">
-        <v>0</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0</v>
-      </c>
-      <c r="I19" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L19" s="5"/>
-      <c r="M19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N19" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-    </row>
-    <row r="20" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="16">
-        <v>25</v>
-      </c>
-      <c r="F20" s="5">
-        <v>1</v>
-      </c>
-      <c r="G20" s="5">
-        <v>0</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0</v>
-      </c>
-      <c r="I20" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N20" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-    </row>
-    <row r="21" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="16">
-        <v>25</v>
-      </c>
-      <c r="F21" s="5">
-        <v>1</v>
-      </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
-        <v>1</v>
-      </c>
-      <c r="I21" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-    </row>
-    <row r="22" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="16">
-        <v>25</v>
-      </c>
-      <c r="F22" s="6">
-        <v>1</v>
-      </c>
-      <c r="G22" s="6">
-        <v>1</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0</v>
-      </c>
-      <c r="I22" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-    </row>
-    <row r="23" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="16">
-        <v>25</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1</v>
-      </c>
-      <c r="G23" s="5">
-        <v>1</v>
-      </c>
-      <c r="H23" s="5">
-        <v>1</v>
-      </c>
-      <c r="I23" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N23" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O23" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-    </row>
-    <row r="24" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="5">
-        <v>1</v>
-      </c>
-      <c r="G24" s="5">
-        <v>0</v>
-      </c>
-      <c r="H24" s="5">
-        <v>0</v>
-      </c>
-      <c r="I24" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N24" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O24" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-    </row>
-    <row r="25" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="5">
-        <v>1</v>
-      </c>
-      <c r="G25" s="5">
-        <v>0</v>
-      </c>
-      <c r="H25" s="5">
-        <v>1</v>
-      </c>
-      <c r="I25" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O25" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-    </row>
-    <row r="26" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="5">
-        <v>1</v>
-      </c>
-      <c r="G26" s="5">
-        <v>1</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0</v>
-      </c>
-      <c r="I26" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K26" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N26" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O26" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-    </row>
-    <row r="27" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1</v>
-      </c>
-      <c r="G27" s="5">
-        <v>1</v>
-      </c>
-      <c r="H27" s="5">
-        <v>1</v>
-      </c>
-      <c r="I27" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K27" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N27" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O27" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-    </row>
-    <row r="28" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F28" s="5">
-        <v>1</v>
-      </c>
-      <c r="G28" s="5">
-        <v>0</v>
-      </c>
-      <c r="H28" s="5">
-        <v>0</v>
-      </c>
-      <c r="I28" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N28" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O28" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-    </row>
-    <row r="29" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F29" s="5">
-        <v>1</v>
-      </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
-      <c r="H29" s="5">
-        <v>1</v>
-      </c>
-      <c r="I29" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K29" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M29" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N29" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O29" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-    </row>
-    <row r="30" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="5">
-        <v>1</v>
-      </c>
-      <c r="G30" s="5">
-        <v>1</v>
-      </c>
-      <c r="H30" s="5">
-        <v>0</v>
-      </c>
-      <c r="I30" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K30" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N30" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O30" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-    </row>
-    <row r="31" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="5">
-        <v>1</v>
-      </c>
-      <c r="G31" s="5">
-        <v>1</v>
-      </c>
-      <c r="H31" s="5">
-        <v>1</v>
-      </c>
-      <c r="I31" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K31" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N31" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O31" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-    </row>
-    <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="16">
-        <v>25</v>
-      </c>
-      <c r="F32" s="5">
-        <v>1</v>
-      </c>
-      <c r="G32" s="5">
-        <v>0</v>
-      </c>
-      <c r="H32" s="5">
-        <v>0</v>
-      </c>
-      <c r="I32" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K32" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N32" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O32" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-    </row>
-    <row r="33" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E33" s="16">
-        <v>25</v>
-      </c>
-      <c r="F33" s="5">
-        <v>1</v>
-      </c>
-      <c r="G33" s="5">
-        <v>0</v>
-      </c>
-      <c r="H33" s="5">
-        <v>1</v>
-      </c>
-      <c r="I33" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K33" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M33" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N33" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O33" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-    </row>
-    <row r="34" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E34" s="16">
-        <v>25</v>
-      </c>
-      <c r="F34" s="5">
-        <v>1</v>
-      </c>
-      <c r="G34" s="5">
-        <v>1</v>
-      </c>
-      <c r="H34" s="5">
-        <v>0</v>
-      </c>
-      <c r="I34" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K34" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M34" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N34" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O34" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-    </row>
-    <row r="35" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" s="16">
-        <v>25</v>
-      </c>
-      <c r="F35" s="5">
-        <v>1</v>
-      </c>
-      <c r="G35" s="5">
-        <v>1</v>
-      </c>
-      <c r="H35" s="5">
-        <v>1</v>
-      </c>
-      <c r="I35" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K35" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N35" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O35" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-    </row>
-    <row r="36" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="6">
-        <v>1</v>
-      </c>
-      <c r="G36" s="6">
-        <v>0</v>
-      </c>
-      <c r="H36" s="6">
-        <v>0</v>
-      </c>
-      <c r="I36" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K36" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M36" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N36" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-    </row>
-    <row r="37" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F37" s="5">
-        <v>1</v>
-      </c>
-      <c r="G37" s="5">
-        <v>0</v>
-      </c>
-      <c r="H37" s="5">
-        <v>0</v>
-      </c>
-      <c r="I37" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K37" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M37" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N37" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O37" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-    </row>
-    <row r="38" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="16">
-        <v>25</v>
-      </c>
-      <c r="F38" s="5">
-        <v>1</v>
-      </c>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
-      <c r="H38" s="5">
-        <v>0</v>
-      </c>
-      <c r="I38" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K38" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L38" s="5"/>
-      <c r="M38" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N38" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O38" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-    </row>
-    <row r="39" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E39" s="16">
-        <v>25</v>
-      </c>
-      <c r="F39" s="5">
-        <v>1</v>
-      </c>
-      <c r="G39" s="5">
-        <v>0</v>
-      </c>
-      <c r="H39" s="5">
-        <v>1</v>
-      </c>
-      <c r="I39" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K39" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L39" s="5"/>
-      <c r="M39" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N39" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O39" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-    </row>
-    <row r="40" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E40" s="16">
-        <v>25</v>
-      </c>
-      <c r="F40" s="5">
-        <v>1</v>
-      </c>
-      <c r="G40" s="5">
-        <v>1</v>
-      </c>
-      <c r="H40" s="5">
-        <v>0</v>
-      </c>
-      <c r="I40" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K40" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L40" s="5"/>
-      <c r="M40" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N40" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O40" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-    </row>
-    <row r="41" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41" s="16">
-        <v>25</v>
-      </c>
-      <c r="F41" s="5">
-        <v>1</v>
-      </c>
-      <c r="G41" s="5">
-        <v>1</v>
-      </c>
-      <c r="H41" s="5">
-        <v>1</v>
-      </c>
-      <c r="I41" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K41" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L41" s="5"/>
-      <c r="M41" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N41" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O41" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-    </row>
-    <row r="42" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="5">
-        <v>1</v>
-      </c>
-      <c r="G42" s="5">
-        <v>0</v>
-      </c>
-      <c r="H42" s="5">
-        <v>0</v>
-      </c>
-      <c r="I42" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L42" s="5"/>
-      <c r="M42" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N42" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O42" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-    </row>
-    <row r="43" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43" s="5">
-        <v>1</v>
-      </c>
-      <c r="G43" s="5">
-        <v>0</v>
-      </c>
-      <c r="H43" s="5">
-        <v>1</v>
-      </c>
-      <c r="I43" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L43" s="5"/>
-      <c r="M43" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N43" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O43" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-    </row>
-    <row r="44" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" s="5">
-        <v>1</v>
-      </c>
-      <c r="G44" s="5">
-        <v>1</v>
-      </c>
-      <c r="H44" s="5">
-        <v>0</v>
-      </c>
-      <c r="I44" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K44" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L44" s="5"/>
-      <c r="M44" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N44" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O44" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-    </row>
-    <row r="45" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F45" s="5">
-        <v>1</v>
-      </c>
-      <c r="G45" s="5">
-        <v>1</v>
-      </c>
-      <c r="H45" s="5">
-        <v>1</v>
-      </c>
-      <c r="I45" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L45" s="5"/>
-      <c r="M45" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N45" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O45" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-    </row>
-    <row r="46" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" s="5">
-        <v>1</v>
-      </c>
-      <c r="G46" s="5">
-        <v>0</v>
-      </c>
-      <c r="H46" s="5">
-        <v>0</v>
-      </c>
-      <c r="I46" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K46" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L46" s="5"/>
-      <c r="M46" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N46" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O46" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-    </row>
-    <row r="47" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="F47" s="5">
-        <v>1</v>
-      </c>
-      <c r="G47" s="5">
-        <v>0</v>
-      </c>
-      <c r="H47" s="5">
-        <v>1</v>
-      </c>
-      <c r="I47" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K47" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L47" s="5"/>
-      <c r="M47" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N47" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O47" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-    </row>
-    <row r="48" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="F48" s="5">
-        <v>1</v>
-      </c>
-      <c r="G48" s="5">
-        <v>1</v>
-      </c>
-      <c r="H48" s="5">
-        <v>0</v>
-      </c>
-      <c r="I48" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K48" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L48" s="5"/>
-      <c r="M48" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N48" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O48" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="5"/>
-    </row>
-    <row r="49" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="F49" s="5">
-        <v>1</v>
-      </c>
-      <c r="G49" s="5">
-        <v>1</v>
-      </c>
-      <c r="H49" s="5">
-        <v>1</v>
-      </c>
-      <c r="I49" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K49" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L49" s="5"/>
-      <c r="M49" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N49" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O49" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-    </row>
-    <row r="50" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E50" s="16">
-        <v>25</v>
-      </c>
-      <c r="F50" s="6">
-        <v>1</v>
-      </c>
-      <c r="G50" s="6">
-        <v>0</v>
-      </c>
-      <c r="H50" s="6">
-        <v>0</v>
-      </c>
-      <c r="I50" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K50" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L50" s="6"/>
-      <c r="M50" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N50" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O50" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-    </row>
-    <row r="51" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E51" s="16">
-        <v>25</v>
-      </c>
-      <c r="F51" s="5">
-        <v>1</v>
-      </c>
-      <c r="G51" s="5">
-        <v>0</v>
-      </c>
-      <c r="H51" s="5">
-        <v>1</v>
-      </c>
-      <c r="I51" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J51" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K51" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L51" s="5"/>
-      <c r="M51" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N51" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O51" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
-    </row>
-    <row r="52" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E52" s="16">
-        <v>25</v>
-      </c>
-      <c r="F52" s="5">
-        <v>1</v>
-      </c>
-      <c r="G52" s="5">
-        <v>1</v>
-      </c>
-      <c r="H52" s="5">
-        <v>0</v>
-      </c>
-      <c r="I52" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J52" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K52" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L52" s="5"/>
-      <c r="M52" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N52" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O52" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-    </row>
-    <row r="53" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E53" s="16">
-        <v>25</v>
-      </c>
-      <c r="F53" s="5">
-        <v>1</v>
-      </c>
-      <c r="G53" s="5">
-        <v>1</v>
-      </c>
-      <c r="H53" s="5">
-        <v>1</v>
-      </c>
-      <c r="I53" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J53" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K53" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L53" s="5"/>
-      <c r="M53" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N53" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O53" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-    </row>
-    <row r="54" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E54" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F54" s="5">
-        <v>1</v>
-      </c>
-      <c r="G54" s="5">
-        <v>0</v>
-      </c>
-      <c r="H54" s="5">
-        <v>0</v>
-      </c>
-      <c r="I54" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J54" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K54" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L54" s="5"/>
-      <c r="M54" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N54" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O54" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P54" s="5"/>
-      <c r="Q54" s="5"/>
-    </row>
-    <row r="55" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F55" s="5">
-        <v>1</v>
-      </c>
-      <c r="G55" s="5">
-        <v>0</v>
-      </c>
-      <c r="H55" s="5">
-        <v>0</v>
-      </c>
-      <c r="I55" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K55" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L55" s="5"/>
-      <c r="M55" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N55" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O55" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P55" s="5"/>
-      <c r="Q55" s="5"/>
-    </row>
-    <row r="56" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E56" s="16">
-        <v>25</v>
-      </c>
-      <c r="F56" s="5">
-        <v>1</v>
-      </c>
-      <c r="G56" s="5">
-        <v>0</v>
-      </c>
-      <c r="H56" s="5">
-        <v>0</v>
-      </c>
-      <c r="I56" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K56" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L56" s="5"/>
-      <c r="M56" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N56" s="8"/>
-      <c r="O56" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="5"/>
-    </row>
-    <row r="57" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E57" s="16">
-        <v>25</v>
-      </c>
-      <c r="F57" s="5">
-        <v>1</v>
-      </c>
-      <c r="G57" s="5">
-        <v>0</v>
-      </c>
-      <c r="H57" s="5">
-        <v>1</v>
-      </c>
-      <c r="I57" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K57" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L57" s="5"/>
-      <c r="M57" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N57" s="8"/>
-      <c r="O57" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P57" s="5"/>
-      <c r="Q57" s="5"/>
-    </row>
-    <row r="58" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E58" s="16">
-        <v>25</v>
-      </c>
-      <c r="F58" s="6">
-        <v>1</v>
-      </c>
-      <c r="G58" s="6">
-        <v>1</v>
-      </c>
-      <c r="H58" s="6">
-        <v>0</v>
-      </c>
-      <c r="I58" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J58" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K58" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L58" s="6"/>
-      <c r="M58" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N58" s="8"/>
-      <c r="O58" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P58" s="5"/>
-      <c r="Q58" s="5"/>
-    </row>
-    <row r="59" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E59" s="16">
-        <v>25</v>
-      </c>
-      <c r="F59" s="5">
-        <v>1</v>
-      </c>
-      <c r="G59" s="5">
-        <v>1</v>
-      </c>
-      <c r="H59" s="5">
-        <v>1</v>
-      </c>
-      <c r="I59" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J59" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K59" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L59" s="5"/>
-      <c r="M59" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N59" s="8"/>
-      <c r="O59" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P59" s="5"/>
-      <c r="Q59" s="5"/>
-    </row>
-    <row r="60" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F60" s="5">
-        <v>1</v>
-      </c>
-      <c r="G60" s="5">
-        <v>0</v>
-      </c>
-      <c r="H60" s="5">
-        <v>0</v>
-      </c>
-      <c r="I60" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L60" s="5"/>
-      <c r="M60" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N60" s="8"/>
-      <c r="O60" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P60" s="5"/>
-      <c r="Q60" s="5"/>
-    </row>
-    <row r="61" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E61" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F61" s="5">
-        <v>1</v>
-      </c>
-      <c r="G61" s="5">
-        <v>0</v>
-      </c>
-      <c r="H61" s="5">
-        <v>1</v>
-      </c>
-      <c r="I61" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K61" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L61" s="5"/>
-      <c r="M61" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N61" s="8"/>
-      <c r="O61" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P61" s="5"/>
-      <c r="Q61" s="5"/>
-    </row>
-    <row r="62" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E62" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F62" s="5">
-        <v>1</v>
-      </c>
-      <c r="G62" s="5">
-        <v>1</v>
-      </c>
-      <c r="H62" s="5">
-        <v>0</v>
-      </c>
-      <c r="I62" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J62" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K62" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L62" s="5"/>
-      <c r="M62" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N62" s="8"/>
-      <c r="O62" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P62" s="5"/>
-      <c r="Q62" s="5"/>
-    </row>
-    <row r="63" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E63" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F63" s="5">
-        <v>1</v>
-      </c>
-      <c r="G63" s="5">
-        <v>1</v>
-      </c>
-      <c r="H63" s="5">
-        <v>1</v>
-      </c>
-      <c r="I63" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J63" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K63" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L63" s="5"/>
-      <c r="M63" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N63" s="8"/>
-      <c r="O63" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P63" s="5"/>
-      <c r="Q63" s="5"/>
-    </row>
-    <row r="64" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F64" s="5">
-        <v>1</v>
-      </c>
-      <c r="G64" s="5">
-        <v>0</v>
-      </c>
-      <c r="H64" s="5">
-        <v>0</v>
-      </c>
-      <c r="I64" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J64" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K64" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L64" s="5"/>
-      <c r="M64" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N64" s="8"/>
-      <c r="O64" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="5"/>
-    </row>
-    <row r="65" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E65" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F65" s="5">
-        <v>1</v>
-      </c>
-      <c r="G65" s="5">
-        <v>0</v>
-      </c>
-      <c r="H65" s="5">
-        <v>1</v>
-      </c>
-      <c r="I65" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K65" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L65" s="5"/>
-      <c r="M65" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N65" s="8"/>
-      <c r="O65" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P65" s="5"/>
-      <c r="Q65" s="5"/>
-    </row>
-    <row r="66" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F66" s="5">
-        <v>1</v>
-      </c>
-      <c r="G66" s="5">
-        <v>1</v>
-      </c>
-      <c r="H66" s="5">
-        <v>0</v>
-      </c>
-      <c r="I66" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J66" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K66" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L66" s="5"/>
-      <c r="M66" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N66" s="8"/>
-      <c r="O66" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P66" s="5"/>
-      <c r="Q66" s="5"/>
-    </row>
-    <row r="67" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E67" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F67" s="5">
-        <v>1</v>
-      </c>
-      <c r="G67" s="5">
-        <v>1</v>
-      </c>
-      <c r="H67" s="5">
-        <v>1</v>
-      </c>
-      <c r="I67" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K67" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L67" s="5"/>
-      <c r="M67" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N67" s="8"/>
-      <c r="O67" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P67" s="5"/>
-      <c r="Q67" s="5"/>
-    </row>
-    <row r="68" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E68" s="16">
-        <v>25</v>
-      </c>
-      <c r="F68" s="5">
-        <v>1</v>
-      </c>
-      <c r="G68" s="5">
-        <v>0</v>
-      </c>
-      <c r="H68" s="5">
-        <v>0</v>
-      </c>
-      <c r="I68" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K68" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L68" s="5"/>
-      <c r="M68" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N68" s="8"/>
-      <c r="O68" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P68" s="5"/>
-      <c r="Q68" s="5"/>
-    </row>
-    <row r="69" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E69" s="16">
-        <v>25</v>
-      </c>
-      <c r="F69" s="5">
-        <v>1</v>
-      </c>
-      <c r="G69" s="5">
-        <v>0</v>
-      </c>
-      <c r="H69" s="5">
-        <v>1</v>
-      </c>
-      <c r="I69" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K69" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L69" s="5"/>
-      <c r="M69" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N69" s="8"/>
-      <c r="O69" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-    </row>
-    <row r="70" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E70" s="16">
-        <v>25</v>
-      </c>
-      <c r="F70" s="5">
-        <v>1</v>
-      </c>
-      <c r="G70" s="5">
-        <v>1</v>
-      </c>
-      <c r="H70" s="5">
-        <v>0</v>
-      </c>
-      <c r="I70" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J70" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K70" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L70" s="5"/>
-      <c r="M70" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N70" s="8"/>
-      <c r="O70" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P70" s="5"/>
-      <c r="Q70" s="5"/>
-    </row>
-    <row r="71" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E71" s="16">
-        <v>25</v>
-      </c>
-      <c r="F71" s="5">
-        <v>1</v>
-      </c>
-      <c r="G71" s="5">
-        <v>1</v>
-      </c>
-      <c r="H71" s="5">
-        <v>1</v>
-      </c>
-      <c r="I71" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J71" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K71" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L71" s="5"/>
-      <c r="M71" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N71" s="8"/>
-      <c r="O71" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P71" s="5"/>
-      <c r="Q71" s="5"/>
-    </row>
-    <row r="72" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E72" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F72" s="6">
-        <v>1</v>
-      </c>
-      <c r="G72" s="6">
-        <v>0</v>
-      </c>
-      <c r="H72" s="6">
-        <v>0</v>
-      </c>
-      <c r="I72" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J72" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K72" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L72" s="6"/>
-      <c r="M72" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N72" s="8"/>
-      <c r="O72" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P72" s="5"/>
-      <c r="Q72" s="5"/>
-    </row>
-    <row r="73" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E73" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F73" s="6">
-        <v>1</v>
-      </c>
-      <c r="G73" s="6">
-        <v>0</v>
-      </c>
-      <c r="H73" s="6">
-        <v>0</v>
-      </c>
-      <c r="I73" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J73" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K73" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L73" s="6"/>
-      <c r="M73" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N73" s="8"/>
-      <c r="O73" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P73" s="6"/>
-      <c r="Q73" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
limited test scenarios for testing purpose and added a preferred cust credentials
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="40">
   <si>
     <t>Description</t>
   </si>
@@ -78,9 +78,6 @@
     <t>AmadeusWS air oneway booking for DOMESTIC location for 1 Adult and 1 child with Login.</t>
   </si>
   <si>
-    <t>AmadeusWS air oneway booking for DOMESTIC location for 1 adult and 1 infant with Login.</t>
-  </si>
-  <si>
     <t>OneWay</t>
   </si>
   <si>
@@ -135,10 +132,10 @@
     <t>Creditcard</t>
   </si>
   <si>
-    <t>Sabre air MULTICITY booking for DOMESTIC location for 1 adult .1 child and 1 infant with On Account payment mode</t>
-  </si>
-  <si>
     <t>Preferred</t>
+  </si>
+  <si>
+    <t>Guest</t>
   </si>
 </sst>
 </file>
@@ -1436,8 +1433,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:Q4" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
-  <autoFilter ref="A1:Q4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+  <autoFilter ref="A1:Q3"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="58"/>
     <tableColumn id="16" name="ExecutionPipeline" dataDxfId="57"/>
@@ -1462,8 +1459,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:Q4" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
-  <autoFilter ref="A1:Q4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+  <autoFilter ref="A1:Q3"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="37"/>
     <tableColumn id="16" name="ExecutionPipeline" dataDxfId="36"/>
@@ -1488,8 +1485,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table234" displayName="Table234" ref="A1:Q4" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="A1:Q4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table234" displayName="Table234" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="A1:Q3"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="16"/>
     <tableColumn id="16" name="ExecutionPipeline" dataDxfId="15"/>
@@ -1800,12 +1797,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+      <selection pane="topRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1876,27 +1873,27 @@
         <v>12</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="5">
         <v>1</v>
@@ -1917,35 +1914,35 @@
         <v>0</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
@@ -1966,73 +1963,24 @@
         <v>0</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1048481">
-      <formula1>$O$1048481:$O$1048487</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1048480">
+      <formula1>$O$1048480:$O$1048486</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2045,10 +1993,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2077,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -2119,10 +2067,10 @@
         <v>12</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
@@ -2130,16 +2078,16 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
@@ -2161,13 +2109,13 @@
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
@@ -2177,10 +2125,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>13</v>
@@ -2208,63 +2156,16 @@
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="14">
-        <v>25</v>
-      </c>
-      <c r="F4" s="10">
-        <v>1</v>
-      </c>
-      <c r="G4" s="10">
-        <v>1</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2276,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2308,7 +2209,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>1</v>
@@ -2350,10 +2251,10 @@
         <v>12</v>
       </c>
       <c r="P1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
@@ -2361,16 +2262,16 @@
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
@@ -2392,13 +2293,13 @@
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
@@ -2408,10 +2309,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>13</v>
@@ -2439,63 +2340,16 @@
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="14">
-        <v>25</v>
-      </c>
-      <c r="F4" s="10">
-        <v>1</v>
-      </c>
-      <c r="G4" s="10">
-        <v>1</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added screen shot methods to test
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/AirScenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="AirLoginRoviaBucks" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Economy</t>
   </si>
   <si>
-    <t>RoviaBucks</t>
-  </si>
-  <si>
     <t>Supplier</t>
   </si>
   <si>
@@ -81,27 +78,9 @@
     <t>Registered</t>
   </si>
   <si>
-    <t>MultiCity</t>
-  </si>
-  <si>
-    <t>Sabre air MULTICITY booking for DOMESTIC location 1 Adult and 1 child with On Account payment mode</t>
-  </si>
-  <si>
     <t>LAS-LAX</t>
   </si>
   <si>
-    <t>Sabre</t>
-  </si>
-  <si>
-    <t>Southwest Airlines</t>
-  </si>
-  <si>
-    <t>LAS-LAX|LAX-DFW|DFW-MIA</t>
-  </si>
-  <si>
-    <t>53|64|71</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -124,6 +103,9 @@
   </si>
   <si>
     <t>Guest</t>
+  </si>
+  <si>
+    <t>Search</t>
   </si>
 </sst>
 </file>
@@ -158,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -260,24 +242,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -300,16 +269,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -333,7 +293,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="64">
+  <dxfs count="63">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1060,81 +1020,237 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1147,160 +1263,8 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1336,24 +1300,42 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1378,9 +1360,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1418,7 +1397,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="58"/>
@@ -1784,10 +1763,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="B11" sqref="B11"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,7 +1775,7 @@
     <col min="2" max="2" width="81.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -1816,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1824,7 +1803,7 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1852,73 +1831,66 @@
         <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>22</v>
+    <row r="2" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="5">
+      <c r="F2" s="6">
         <v>1</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="5">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6" t="b">
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11" t="b">
         <v>0</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="5" t="b">
+      <c r="K2" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="L2" s="7"/>
       <c r="M2" s="8" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1048479">
-      <formula1>$O$1048479:$O$1048485</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1932,7 +1904,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,9 +1917,9 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1"/>
@@ -1961,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1969,7 +1941,7 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1981,13 +1953,13 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -1997,33 +1969,33 @@
         <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
@@ -2034,27 +2006,27 @@
       <c r="H2" s="6">
         <v>0</v>
       </c>
-      <c r="I2" s="14" t="b">
+      <c r="I2" s="11" t="b">
         <v>0</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="14" t="b">
+      <c r="K2" s="11" t="b">
         <v>0</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
+        <v>19</v>
+      </c>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2068,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,9 +2054,9 @@
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
@@ -2094,73 +2066,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="17" t="s">
+      <c r="N1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="17" t="s">
-        <v>31</v>
+      <c r="P1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
@@ -2171,27 +2143,27 @@
       <c r="H2" s="6">
         <v>0</v>
       </c>
-      <c r="I2" s="14" t="b">
+      <c r="I2" s="11" t="b">
         <v>0</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="14" t="b">
+      <c r="K2" s="11" t="b">
         <v>0</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
+        <v>28</v>
+      </c>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>